<commit_message>
update order list and power supply
</commit_message>
<xml_diff>
--- a/Seminar_Med_Tech/Conrad_offen_NN2.xlsx
+++ b/Seminar_Med_Tech/Conrad_offen_NN2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isshu\Documents\Seminar_Medizintechnik\Seminar_Med_Tech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TsEric/Documents/Seminar_Medizintechnik/Seminar_Med_Tech/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595" tabRatio="4"/>
+    <workbookView xWindow="940" yWindow="440" windowWidth="20500" windowHeight="8600" tabRatio="4"/>
   </bookViews>
   <sheets>
     <sheet name="Bestellung-Conrad" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,15 @@
     <definedName name="head_detail" localSheetId="1">'[3]Bestellung-Reichelt'!#REF!</definedName>
     <definedName name="head_detail">'Bestellung-Conrad'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -228,17 +236,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="9">
-    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="172" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* \-??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="[$€]#,##0.00\ ;[$€]\(#,##0.00\);[$€]\-#\ ;@\ "/>
-    <numFmt numFmtId="174" formatCode="#,##0.00\ [$€-407];[Red]\-#,##0.00\ [$€-407]"/>
-    <numFmt numFmtId="175" formatCode="#,##0.00\ [$€-407]"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00&quot; €&quot;_-;\-* #,##0.00&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00&quot; €&quot;;[Red]\-#,##0.00&quot; €&quot;"/>
-    <numFmt numFmtId="187" formatCode="#,##0.00&quot; €&quot;"/>
-    <numFmt numFmtId="188" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* \-??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$€]#,##0.00\ ;[$€]\(#,##0.00\);[$€]\-#\ ;@\ "/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ [$€-407];[Red]\-#,##0.00\ [$€-407]"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ [$€-407]"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.00&quot; €&quot;_-;\-* #,##0.00&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00&quot; €&quot;;[Red]\-#,##0.00&quot; €&quot;"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00&quot; €&quot;"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
   <fonts count="43" x14ac:knownFonts="1">
     <font>
@@ -834,7 +842,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -936,9 +944,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="31" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="173" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -984,9 +992,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="188" fontId="40" fillId="0" borderId="0"/>
-    <xf numFmtId="174" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="174" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="172" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0"/>
@@ -1035,10 +1043,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="15" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1059,10 +1067,10 @@
       <alignment shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="7" fillId="8" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="7" fillId="8" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
@@ -1079,24 +1087,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="7" fillId="0" borderId="0" xfId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="164" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="7" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="164" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="164" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1107,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1120,10 +1128,10 @@
     <xf numFmtId="0" fontId="29" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="175" fontId="29" fillId="27" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="29" fillId="27" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="34" fillId="27" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="34" fillId="27" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1136,22 +1144,22 @@
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="27" fillId="29" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="27" fillId="29" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="175" fontId="28" fillId="29" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="28" fillId="29" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="28" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="31" fillId="29" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="31" fillId="29" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="7" fillId="29" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="7" fillId="29" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1170,10 +1178,10 @@
     <xf numFmtId="0" fontId="29" fillId="8" borderId="10" xfId="122" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="175" fontId="29" fillId="8" borderId="10" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="29" fillId="8" borderId="10" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="34" fillId="8" borderId="10" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="34" fillId="8" borderId="10" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1185,27 +1193,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="122" applyFont="1"/>
-    <xf numFmtId="174" fontId="7" fillId="0" borderId="0" xfId="166" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="166" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="29" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="32" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="32" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="122" applyBorder="1"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="166" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="166" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="122" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="122" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1215,13 +1223,13 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="122" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="129" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="122" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
@@ -1244,10 +1252,10 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="122" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="122" applyFont="1"/>
@@ -1258,12 +1266,12 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="122" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" xfId="122" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="42" fillId="31" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1344,6 +1352,7 @@
     <cellStyle name="Berechnung 2" xfId="58"/>
     <cellStyle name="Berechnung 2 2" xfId="59"/>
     <cellStyle name="Berechnung 2 3" xfId="60"/>
+    <cellStyle name="Currency" xfId="164" builtinId="4"/>
     <cellStyle name="Default 1" xfId="61"/>
     <cellStyle name="Eingabe 2" xfId="62"/>
     <cellStyle name="Eingabe 2 2" xfId="63"/>
@@ -1381,13 +1390,14 @@
     <cellStyle name="Hinweis" xfId="95"/>
     <cellStyle name="Hinweis 2" xfId="96"/>
     <cellStyle name="Hinweis 3" xfId="97"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="99"/>
     <cellStyle name="Hyperlink 3" xfId="100"/>
-    <cellStyle name="Link" xfId="98" builtinId="8"/>
     <cellStyle name="Link 2" xfId="101"/>
     <cellStyle name="Neutral 2" xfId="102"/>
     <cellStyle name="Neutral 2 2" xfId="103"/>
     <cellStyle name="Neutral 2 3" xfId="104"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notiz 2" xfId="105"/>
     <cellStyle name="Notiz 2 2" xfId="106"/>
     <cellStyle name="Notiz 2 3" xfId="107"/>
@@ -1403,7 +1413,6 @@
     <cellStyle name="Schlecht 2" xfId="117"/>
     <cellStyle name="Schlecht 2 2" xfId="118"/>
     <cellStyle name="Schlecht 2 3" xfId="119"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="120"/>
     <cellStyle name="Standard 2 2" xfId="121"/>
     <cellStyle name="Standard 2 3" xfId="122"/>
@@ -1448,7 +1457,6 @@
     <cellStyle name="Verknüpfte Zelle 2" xfId="161"/>
     <cellStyle name="Verknüpfte Zelle 2 2" xfId="162"/>
     <cellStyle name="Verknüpfte Zelle 2 3" xfId="163"/>
-    <cellStyle name="Währung" xfId="164" builtinId="4"/>
     <cellStyle name="Währung 2" xfId="165"/>
     <cellStyle name="Währung 3" xfId="166"/>
     <cellStyle name="Währung 4" xfId="167"/>
@@ -2604,23 +2612,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="C8" activeCellId="1" sqref="A9 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="3" max="3" width="56.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2635,14 +2643,14 @@
       <c r="E1" s="32"/>
       <c r="F1" s="34"/>
     </row>
-    <row r="2" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="79">
         <f ca="1">IF(C1&gt;=0,NOW(),0)</f>
-        <v>42907.624422685185</v>
+        <v>42907.69143136574</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="37" t="s">
@@ -2650,10 +2658,10 @@
       </c>
       <c r="F2" s="79">
         <f ca="1">IF(F1&gt;=0,NOW(),0)</f>
-        <v>42907.624422685185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>42907.69143136574</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="83" t="s">
         <v>21</v>
       </c>
@@ -2665,7 +2673,7 @@
       <c r="E3" s="37"/>
       <c r="F3" s="39"/>
     </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="84"/>
       <c r="B4" s="84"/>
       <c r="C4" s="82" t="s">
@@ -2675,7 +2683,7 @@
       <c r="E4" s="37"/>
       <c r="F4" s="39"/>
     </row>
-    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="84"/>
       <c r="B5" s="84"/>
       <c r="C5" s="81" t="s">
@@ -2685,20 +2693,20 @@
       <c r="E5" s="37"/>
       <c r="F5" s="39"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="31"/>
       <c r="C6" s="40" t="str">
         <f>COUNT(A:A)&amp;" / "&amp;SUM(A:A)</f>
-        <v>0 / 0</v>
+        <v>1 / 10</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="37"/>
       <c r="F6" s="40"/>
     </row>
-    <row r="7" spans="1:6" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="24" t="s">
         <v>4</v>
       </c>
@@ -2718,12 +2726,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13" t="str">
         <f>IF(ISNUMBER(A8),IF(A8&gt;=0,IF(D8&gt;=0,D8*A8,0),""),"")</f>
@@ -2734,9 +2744,9 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>27</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="10">
+        <v>10</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>25</v>
@@ -2751,17 +2761,17 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
       <c r="E10" s="17" t="str">
-        <f t="shared" ref="E9:E71" si="0">IF(ISNUMBER(A10),IF(A10&gt;=0,IF(D10&gt;=0,D10*A10,0),""),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="E10:E71" si="0">IF(ISNUMBER(A10),IF(A10&gt;=0,IF(D10&gt;=0,D10*A10,0),""),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11"/>
@@ -2771,7 +2781,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -2781,7 +2791,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -2792,7 +2802,7 @@
       </c>
       <c r="F13" s="16"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -2802,7 +2812,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -2812,7 +2822,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -2822,7 +2832,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
@@ -2832,7 +2842,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
@@ -2843,7 +2853,7 @@
       </c>
       <c r="F18" s="16"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
@@ -2853,7 +2863,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20"/>
@@ -2863,7 +2873,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21"/>
@@ -2874,7 +2884,7 @@
       </c>
       <c r="F21" s="23"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22"/>
@@ -2884,7 +2894,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23"/>
@@ -2894,7 +2904,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24"/>
@@ -2904,7 +2914,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25"/>
@@ -2914,7 +2924,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -2925,7 +2935,7 @@
       </c>
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
@@ -2935,7 +2945,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
@@ -2945,7 +2955,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
@@ -2955,7 +2965,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
@@ -2965,7 +2975,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
@@ -2975,7 +2985,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
@@ -2985,7 +2995,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
@@ -2995,7 +3005,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
@@ -3005,7 +3015,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35"/>
@@ -3015,7 +3025,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36"/>
@@ -3025,7 +3035,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37"/>
@@ -3035,7 +3045,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38"/>
@@ -3045,7 +3055,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39"/>
@@ -3055,7 +3065,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40"/>
@@ -3065,7 +3075,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
@@ -3076,7 +3086,7 @@
       </c>
       <c r="F41" s="16"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
@@ -3087,7 +3097,7 @@
       </c>
       <c r="F42" s="16"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
@@ -3097,7 +3107,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44"/>
@@ -3107,7 +3117,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45"/>
@@ -3117,7 +3127,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46"/>
@@ -3127,7 +3137,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="11"/>
@@ -3137,7 +3147,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="11"/>
@@ -3147,7 +3157,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
       <c r="C49" s="11"/>
@@ -3157,7 +3167,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" s="10"/>
       <c r="B50" s="10"/>
       <c r="C50" s="11"/>
@@ -3167,7 +3177,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
@@ -3177,7 +3187,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
@@ -3187,7 +3197,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
       <c r="C53"/>
@@ -3197,7 +3207,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54"/>
@@ -3207,7 +3217,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55"/>
@@ -3217,7 +3227,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56"/>
@@ -3227,7 +3237,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
       <c r="C57"/>
@@ -3237,7 +3247,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58"/>
@@ -3247,7 +3257,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59"/>
@@ -3257,7 +3267,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60"/>
@@ -3269,7 +3279,7 @@
       <c r="F60" s="19"/>
       <c r="G60" s="19"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61"/>
@@ -3279,7 +3289,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" s="10"/>
       <c r="B62" s="10"/>
       <c r="C62" s="21"/>
@@ -3289,7 +3299,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="21"/>
@@ -3299,7 +3309,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="21"/>
@@ -3309,7 +3319,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="11"/>
@@ -3319,7 +3329,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
@@ -3329,7 +3339,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
@@ -3342,7 +3352,7 @@
       <c r="G67" s="22"/>
       <c r="H67" s="22"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="11"/>
@@ -3355,7 +3365,7 @@
       <c r="G68" s="22"/>
       <c r="H68" s="22"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="11"/>
@@ -3365,7 +3375,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
@@ -3375,7 +3385,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
@@ -3385,7 +3395,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
       <c r="C72" s="11"/>
@@ -3395,7 +3405,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
       <c r="C73" s="11"/>
@@ -3405,7 +3415,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
       <c r="C74" s="11"/>
@@ -3415,7 +3425,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
@@ -3425,7 +3435,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="11"/>
@@ -3435,7 +3445,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A77" s="10"/>
       <c r="B77" s="10"/>
       <c r="C77"/>
@@ -3445,7 +3455,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
       <c r="C78"/>
@@ -3455,7 +3465,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79"/>
@@ -3465,7 +3475,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
       <c r="C80"/>
@@ -3475,7 +3485,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81"/>
@@ -3485,7 +3495,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82"/>
@@ -3495,7 +3505,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="11"/>
@@ -3505,7 +3515,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="11"/>
@@ -3515,7 +3525,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="11"/>
@@ -3525,7 +3535,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="11"/>
@@ -3535,7 +3545,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="11"/>
@@ -3545,7 +3555,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="11"/>
@@ -3555,7 +3565,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89"/>
@@ -3565,7 +3575,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90"/>
@@ -3575,7 +3585,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91"/>
@@ -3585,7 +3595,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
       <c r="C92" s="11"/>
@@ -3595,7 +3605,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
       <c r="C93" s="11"/>
@@ -3605,7 +3615,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
       <c r="C94" s="11"/>
@@ -3615,7 +3625,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95"/>
@@ -3625,7 +3635,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="8"/>
       <c r="B96" s="20"/>
       <c r="C96"/>
@@ -3635,7 +3645,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A97" s="8"/>
       <c r="B97" s="20"/>
       <c r="C97"/>
@@ -3645,7 +3655,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A98" s="8"/>
       <c r="B98" s="20"/>
       <c r="C98"/>
@@ -3655,7 +3665,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A99" s="8"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -3665,7 +3675,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A100" s="8"/>
       <c r="B100" s="20"/>
       <c r="C100"/>
@@ -3675,7 +3685,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A101" s="8"/>
       <c r="B101" s="20"/>
       <c r="C101"/>
@@ -3686,7 +3696,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="A3:B3"/>
@@ -3835,15 +3844,15 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="47" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="47" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="47" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="47"/>
+    <col min="1" max="1" width="10.33203125" style="47" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="47" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="47" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
         <v>4</v>
       </c>
@@ -3863,7 +3872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="48" t="s">
         <v>14</v>
       </c>
@@ -3876,7 +3885,7 @@
       </c>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="54" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="48">
         <v>100</v>
       </c>
@@ -3895,7 +3904,7 @@
       </c>
       <c r="F3" s="53"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="48"/>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
@@ -3906,47 +3915,47 @@
       </c>
       <c r="F4" s="53"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="48"/>
       <c r="B5" s="48"/>
       <c r="D5" s="55"/>
       <c r="E5" s="13"/>
       <c r="F5" s="53"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D6" s="56"/>
       <c r="E6" s="13"/>
       <c r="F6" s="53"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D7" s="56"/>
       <c r="E7" s="13"/>
       <c r="F7" s="53"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D8" s="56"/>
       <c r="E8" s="13"/>
       <c r="F8" s="53"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B9" s="57"/>
       <c r="D9" s="58"/>
       <c r="E9" s="13"/>
       <c r="F9" s="53"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B10" s="59"/>
       <c r="D10" s="58"/>
       <c r="E10" s="13"/>
       <c r="F10" s="53"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B11" s="57"/>
       <c r="D11" s="58"/>
       <c r="E11" s="13"/>
       <c r="F11" s="53"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="48"/>
       <c r="B12" s="48"/>
       <c r="C12" s="49"/>
@@ -3954,7 +3963,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="53"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="60"/>
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
@@ -3962,7 +3971,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="53"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="60"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
@@ -3970,7 +3979,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="53"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="60"/>
       <c r="B15" s="49"/>
       <c r="C15" s="49"/>
@@ -3978,7 +3987,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="53"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="60"/>
       <c r="B16" s="49"/>
       <c r="C16" s="49"/>
@@ -3986,7 +3995,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="53"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="60"/>
       <c r="B17" s="49"/>
       <c r="C17" s="49"/>
@@ -3994,7 +4003,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="53"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="60"/>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
@@ -4002,7 +4011,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="53"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="60"/>
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
@@ -4010,7 +4019,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="53"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="60"/>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
@@ -4018,7 +4027,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="53"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="48"/>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
@@ -4026,7 +4035,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="61"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="48"/>
       <c r="B22" s="48"/>
       <c r="C22" s="49"/>
@@ -4034,7 +4043,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="61"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="48"/>
       <c r="B23" s="48"/>
       <c r="C23" s="49"/>
@@ -4042,7 +4051,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="61"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="48"/>
       <c r="B24" s="48"/>
       <c r="C24" s="49"/>
@@ -4050,49 +4059,49 @@
       <c r="E24" s="13"/>
       <c r="F24" s="61"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="48"/>
       <c r="B25" s="48"/>
       <c r="D25" s="55"/>
       <c r="E25" s="13"/>
       <c r="F25" s="61"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="48"/>
       <c r="B26" s="48"/>
       <c r="D26" s="55"/>
       <c r="E26" s="13"/>
       <c r="F26" s="61"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="48"/>
       <c r="B27" s="48"/>
       <c r="D27" s="55"/>
       <c r="E27" s="13"/>
       <c r="F27" s="61"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="48"/>
       <c r="B28" s="48"/>
       <c r="D28" s="55"/>
       <c r="E28" s="13"/>
       <c r="F28" s="61"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="48"/>
       <c r="B29" s="48"/>
       <c r="D29" s="55"/>
       <c r="E29" s="13"/>
       <c r="F29" s="61"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="48"/>
       <c r="B30" s="48"/>
       <c r="D30" s="55"/>
       <c r="E30" s="13"/>
       <c r="F30" s="61"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="48"/>
       <c r="B31" s="48"/>
       <c r="C31" s="49"/>
@@ -4100,7 +4109,7 @@
       <c r="E31" s="13"/>
       <c r="F31" s="61"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="48"/>
       <c r="B32" s="48"/>
       <c r="C32" s="49"/>
@@ -4108,7 +4117,7 @@
       <c r="E32" s="13"/>
       <c r="F32" s="61"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="48"/>
       <c r="B33" s="48"/>
       <c r="C33" s="49"/>
@@ -4116,7 +4125,7 @@
       <c r="E33" s="13"/>
       <c r="F33" s="61"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="48"/>
       <c r="B34" s="48"/>
       <c r="C34" s="49"/>
@@ -4124,7 +4133,7 @@
       <c r="E34" s="13"/>
       <c r="F34" s="61"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="48"/>
       <c r="B35" s="48"/>
       <c r="C35" s="49"/>
@@ -4132,7 +4141,7 @@
       <c r="E35" s="13"/>
       <c r="F35" s="61"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="48"/>
       <c r="B36" s="48"/>
       <c r="C36" s="49"/>
@@ -4140,7 +4149,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="61"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="48"/>
       <c r="B37" s="48"/>
       <c r="C37" s="49"/>
@@ -4148,7 +4157,7 @@
       <c r="E37" s="13"/>
       <c r="F37" s="62"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="48"/>
       <c r="B38" s="48"/>
       <c r="C38" s="49"/>
@@ -4156,7 +4165,7 @@
       <c r="E38" s="13"/>
       <c r="F38" s="61"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="48"/>
       <c r="B39" s="48"/>
       <c r="C39" s="49"/>
@@ -4164,49 +4173,49 @@
       <c r="E39" s="13"/>
       <c r="F39" s="61"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="48"/>
       <c r="B40" s="48"/>
       <c r="D40" s="55"/>
       <c r="E40" s="13"/>
       <c r="F40" s="61"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="48"/>
       <c r="B41" s="48"/>
       <c r="D41" s="55"/>
       <c r="E41" s="13"/>
       <c r="F41" s="61"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="48"/>
       <c r="B42" s="48"/>
       <c r="D42" s="55"/>
       <c r="E42" s="13"/>
       <c r="F42" s="61"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="48"/>
       <c r="B43" s="48"/>
       <c r="D43" s="55"/>
       <c r="E43" s="13"/>
       <c r="F43" s="61"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="48"/>
       <c r="B44" s="48"/>
       <c r="D44" s="55"/>
       <c r="E44" s="13"/>
       <c r="F44" s="61"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="48"/>
       <c r="B45" s="48"/>
       <c r="D45" s="55"/>
       <c r="E45" s="13"/>
       <c r="F45" s="61"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="48"/>
       <c r="B46" s="48"/>
       <c r="C46" s="49"/>
@@ -4214,7 +4223,7 @@
       <c r="E46" s="13"/>
       <c r="F46" s="61"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="48"/>
       <c r="B47" s="48"/>
       <c r="C47" s="49"/>
@@ -4222,7 +4231,7 @@
       <c r="E47" s="13"/>
       <c r="F47" s="61"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="48"/>
       <c r="B48" s="48"/>
       <c r="C48" s="49"/>
@@ -4230,28 +4239,28 @@
       <c r="E48" s="13"/>
       <c r="F48" s="61"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="48"/>
       <c r="B49" s="48"/>
       <c r="D49" s="55"/>
       <c r="E49" s="13"/>
       <c r="F49" s="61"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="48"/>
       <c r="B50" s="48"/>
       <c r="D50" s="55"/>
       <c r="E50" s="13"/>
       <c r="F50" s="61"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="48"/>
       <c r="B51" s="48"/>
       <c r="D51" s="55"/>
       <c r="E51" s="13"/>
       <c r="F51" s="61"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="48"/>
       <c r="B52" s="48"/>
       <c r="C52" s="49"/>
@@ -4259,7 +4268,7 @@
       <c r="E52" s="13"/>
       <c r="F52" s="61"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" s="48"/>
       <c r="B53" s="48"/>
       <c r="C53" s="49"/>
@@ -4267,7 +4276,7 @@
       <c r="E53" s="13"/>
       <c r="F53" s="61"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="48"/>
       <c r="B54" s="48"/>
       <c r="C54" s="49"/>
@@ -4275,7 +4284,7 @@
       <c r="E54" s="13"/>
       <c r="F54" s="61"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="48"/>
       <c r="B55" s="48"/>
       <c r="C55" s="49"/>
@@ -4283,7 +4292,7 @@
       <c r="E55" s="13"/>
       <c r="F55" s="61"/>
     </row>
-    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="48"/>
       <c r="B56" s="48"/>
       <c r="C56" s="49"/>
@@ -4291,7 +4300,7 @@
       <c r="E56" s="13"/>
       <c r="F56" s="63"/>
     </row>
-    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="48"/>
       <c r="B57" s="48"/>
       <c r="C57" s="49"/>
@@ -4299,70 +4308,70 @@
       <c r="E57" s="13"/>
       <c r="F57" s="63"/>
     </row>
-    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="48"/>
       <c r="B58" s="48"/>
       <c r="D58" s="64"/>
       <c r="E58" s="13"/>
       <c r="F58" s="63"/>
     </row>
-    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="48"/>
       <c r="B59" s="48"/>
       <c r="D59" s="64"/>
       <c r="E59" s="13"/>
       <c r="F59" s="63"/>
     </row>
-    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="48"/>
       <c r="B60" s="48"/>
       <c r="D60" s="64"/>
       <c r="E60" s="13"/>
       <c r="F60" s="63"/>
     </row>
-    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="48"/>
       <c r="B61" s="48"/>
       <c r="D61" s="64"/>
       <c r="E61" s="13"/>
       <c r="F61" s="63"/>
     </row>
-    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="48"/>
       <c r="B62" s="48"/>
       <c r="D62" s="64"/>
       <c r="E62" s="13"/>
       <c r="F62" s="63"/>
     </row>
-    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="48"/>
       <c r="B63" s="48"/>
       <c r="D63" s="64"/>
       <c r="E63" s="52"/>
       <c r="F63" s="63"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" s="48"/>
       <c r="B64" s="48"/>
       <c r="D64" s="64"/>
       <c r="E64" s="13"/>
       <c r="F64" s="61"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" s="48"/>
       <c r="B65" s="48"/>
       <c r="D65" s="64"/>
       <c r="E65" s="52"/>
       <c r="F65" s="61"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" s="48"/>
       <c r="B66" s="48"/>
       <c r="D66" s="64"/>
       <c r="E66" s="52"/>
       <c r="F66" s="61"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" s="48"/>
       <c r="B67" s="48"/>
       <c r="C67" s="65"/>
@@ -4370,7 +4379,7 @@
       <c r="E67" s="13"/>
       <c r="F67" s="61"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" s="48"/>
       <c r="B68" s="48"/>
       <c r="C68" s="65"/>
@@ -4378,7 +4387,7 @@
       <c r="E68" s="13"/>
       <c r="F68" s="61"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" s="48"/>
       <c r="B69" s="48"/>
       <c r="C69" s="65"/>
@@ -4386,7 +4395,7 @@
       <c r="E69" s="13"/>
       <c r="F69" s="61"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="48"/>
       <c r="B70" s="48"/>
       <c r="C70" s="49"/>
@@ -4394,7 +4403,7 @@
       <c r="E70" s="13"/>
       <c r="F70" s="61"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="48"/>
       <c r="B71" s="66"/>
       <c r="C71" s="66"/>
@@ -4402,7 +4411,7 @@
       <c r="E71" s="13"/>
       <c r="F71" s="61"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" s="48"/>
       <c r="B72" s="66"/>
       <c r="C72" s="66"/>
@@ -4410,7 +4419,7 @@
       <c r="E72" s="13"/>
       <c r="F72" s="61"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" s="48"/>
       <c r="B73" s="48"/>
       <c r="C73" s="48"/>
@@ -4418,7 +4427,7 @@
       <c r="E73" s="13"/>
       <c r="F73" s="48"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" s="48"/>
       <c r="B74" s="48"/>
       <c r="C74" s="49"/>
@@ -4426,7 +4435,7 @@
       <c r="E74" s="13"/>
       <c r="F74" s="61"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="48"/>
       <c r="B75" s="48"/>
       <c r="C75" s="49"/>
@@ -4434,7 +4443,7 @@
       <c r="E75" s="13"/>
       <c r="F75" s="61"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" s="48"/>
       <c r="B76" s="48"/>
       <c r="C76" s="49"/>
@@ -4442,7 +4451,7 @@
       <c r="E76" s="13"/>
       <c r="F76" s="61"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" s="48"/>
       <c r="B77" s="48"/>
       <c r="C77" s="49"/>
@@ -4450,7 +4459,7 @@
       <c r="E77" s="13"/>
       <c r="F77" s="61"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" s="48"/>
       <c r="B78" s="48"/>
       <c r="C78" s="49"/>
@@ -4458,7 +4467,7 @@
       <c r="E78" s="13"/>
       <c r="F78" s="61"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="48"/>
       <c r="B79" s="48"/>
       <c r="C79" s="49"/>
@@ -4466,7 +4475,7 @@
       <c r="E79" s="13"/>
       <c r="F79" s="61"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" s="48"/>
       <c r="B80" s="48"/>
       <c r="C80" s="49"/>
@@ -4474,7 +4483,7 @@
       <c r="E80" s="13"/>
       <c r="F80" s="61"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" s="48"/>
       <c r="B81" s="48"/>
       <c r="C81" s="49"/>
@@ -4482,7 +4491,7 @@
       <c r="E81" s="13"/>
       <c r="F81" s="61"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" s="48"/>
       <c r="B82" s="48"/>
       <c r="C82" s="49"/>
@@ -4490,7 +4499,7 @@
       <c r="E82" s="13"/>
       <c r="F82" s="61"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" s="48"/>
       <c r="B83" s="48"/>
       <c r="C83" s="49"/>
@@ -4498,7 +4507,7 @@
       <c r="E83" s="13"/>
       <c r="F83" s="61"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" s="48"/>
       <c r="B84" s="48"/>
       <c r="C84" s="49"/>
@@ -4506,49 +4515,49 @@
       <c r="E84" s="13"/>
       <c r="F84" s="61"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" s="48"/>
       <c r="B85" s="48"/>
       <c r="D85" s="55"/>
       <c r="E85" s="13"/>
       <c r="F85" s="61"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" s="48"/>
       <c r="B86" s="48"/>
       <c r="D86" s="55"/>
       <c r="E86" s="13"/>
       <c r="F86" s="61"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" s="48"/>
       <c r="B87" s="48"/>
       <c r="D87" s="55"/>
       <c r="E87" s="13"/>
       <c r="F87" s="61"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" s="48"/>
       <c r="B88" s="48"/>
       <c r="D88" s="55"/>
       <c r="E88" s="13"/>
       <c r="F88" s="61"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" s="48"/>
       <c r="B89" s="48"/>
       <c r="D89" s="55"/>
       <c r="E89" s="13"/>
       <c r="F89" s="61"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" s="48"/>
       <c r="B90" s="48"/>
       <c r="D90" s="55"/>
       <c r="E90" s="13"/>
       <c r="F90" s="61"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" s="48"/>
       <c r="B91" s="48"/>
       <c r="C91" s="49"/>
@@ -4556,7 +4565,7 @@
       <c r="E91" s="13"/>
       <c r="F91" s="61"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" s="48"/>
       <c r="B92" s="48"/>
       <c r="C92" s="49"/>
@@ -4564,7 +4573,7 @@
       <c r="E92" s="13"/>
       <c r="F92" s="61"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" s="48"/>
       <c r="B93" s="48"/>
       <c r="C93" s="49"/>
@@ -4572,7 +4581,7 @@
       <c r="E93" s="13"/>
       <c r="F93" s="61"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" s="48"/>
       <c r="B94" s="48"/>
       <c r="C94" s="49"/>
@@ -4580,7 +4589,7 @@
       <c r="E94" s="13"/>
       <c r="F94" s="61"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" s="48"/>
       <c r="B95" s="48"/>
       <c r="C95" s="49"/>
@@ -4588,7 +4597,7 @@
       <c r="E95" s="13"/>
       <c r="F95" s="61"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96" s="48"/>
       <c r="B96" s="48"/>
       <c r="C96" s="49"/>
@@ -4596,28 +4605,28 @@
       <c r="E96" s="13"/>
       <c r="F96" s="61"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" s="48"/>
       <c r="B97" s="48"/>
       <c r="D97" s="55"/>
       <c r="E97" s="13"/>
       <c r="F97" s="61"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98" s="48"/>
       <c r="B98" s="48"/>
       <c r="D98" s="55"/>
       <c r="E98" s="13"/>
       <c r="F98" s="61"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" s="48"/>
       <c r="B99" s="48"/>
       <c r="D99" s="55"/>
       <c r="E99" s="13"/>
       <c r="F99" s="61"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100" s="48"/>
       <c r="B100" s="48"/>
       <c r="C100" s="49"/>
@@ -4625,7 +4634,7 @@
       <c r="E100" s="13"/>
       <c r="F100" s="61"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101" s="48"/>
       <c r="B101" s="48"/>
       <c r="C101" s="49"/>
@@ -4633,7 +4642,7 @@
       <c r="E101" s="13"/>
       <c r="F101" s="61"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102" s="48"/>
       <c r="B102" s="48"/>
       <c r="C102" s="49"/>
@@ -4641,83 +4650,83 @@
       <c r="E102" s="13"/>
       <c r="F102" s="61"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103" s="48"/>
       <c r="B103" s="48"/>
       <c r="D103" s="55"/>
       <c r="E103" s="13"/>
       <c r="F103" s="61"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104" s="67"/>
       <c r="B104" s="68"/>
       <c r="D104" s="55"/>
       <c r="E104" s="13"/>
       <c r="F104" s="61"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" s="67"/>
       <c r="B105" s="68"/>
       <c r="D105" s="55"/>
       <c r="E105" s="13"/>
       <c r="F105" s="61"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A106" s="67"/>
       <c r="B106" s="68"/>
       <c r="D106" s="55"/>
       <c r="E106" s="13"/>
       <c r="F106" s="61"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" s="67"/>
       <c r="D107" s="55"/>
       <c r="E107" s="13"/>
       <c r="F107" s="61"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A108" s="67"/>
       <c r="B108" s="68"/>
       <c r="D108" s="55"/>
       <c r="E108" s="13"/>
       <c r="F108" s="61"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A109" s="67"/>
       <c r="B109" s="68"/>
       <c r="D109" s="55"/>
       <c r="E109" s="13"/>
       <c r="F109" s="61"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A110" s="67"/>
       <c r="B110" s="68"/>
       <c r="D110" s="55"/>
       <c r="E110" s="13"/>
       <c r="F110" s="61"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A111" s="67"/>
       <c r="B111" s="68"/>
       <c r="D111" s="55"/>
       <c r="E111" s="13"/>
       <c r="F111" s="61"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A112" s="67"/>
       <c r="B112" s="68"/>
       <c r="D112" s="55"/>
       <c r="E112" s="13"/>
       <c r="F112" s="61"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" s="67"/>
       <c r="B113" s="68"/>
       <c r="D113" s="55"/>
       <c r="E113" s="13"/>
       <c r="F113" s="61"/>
     </row>
-    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="69"/>
       <c r="B114" s="70"/>
       <c r="C114" s="71"/>
@@ -4725,7 +4734,7 @@
       <c r="E114" s="73"/>
       <c r="F114" s="61"/>
     </row>
-    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="69"/>
       <c r="B115" s="70"/>
       <c r="C115" s="71"/>
@@ -4733,7 +4742,7 @@
       <c r="E115" s="73"/>
       <c r="F115" s="61"/>
     </row>
-    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="69"/>
       <c r="B116" s="70"/>
       <c r="C116" s="71"/>
@@ -4741,7 +4750,7 @@
       <c r="E116" s="73"/>
       <c r="F116" s="61"/>
     </row>
-    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="69"/>
       <c r="B117" s="70"/>
       <c r="C117" s="71"/>
@@ -4749,7 +4758,7 @@
       <c r="E117" s="73"/>
       <c r="F117" s="61"/>
     </row>
-    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="69"/>
       <c r="B118" s="70"/>
       <c r="C118" s="71"/>
@@ -4757,7 +4766,7 @@
       <c r="E118" s="73"/>
       <c r="F118" s="61"/>
     </row>
-    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="69"/>
       <c r="B119" s="70"/>
       <c r="C119" s="71"/>
@@ -4765,7 +4774,7 @@
       <c r="E119" s="73"/>
       <c r="F119" s="61"/>
     </row>
-    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="69"/>
       <c r="B120" s="70"/>
       <c r="C120" s="71"/>
@@ -4773,7 +4782,7 @@
       <c r="E120" s="73"/>
       <c r="F120" s="61"/>
     </row>
-    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="69"/>
       <c r="B121" s="70"/>
       <c r="C121" s="71"/>
@@ -4781,7 +4790,7 @@
       <c r="E121" s="73"/>
       <c r="F121" s="61"/>
     </row>
-    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="69"/>
       <c r="B122" s="70"/>
       <c r="C122" s="71"/>
@@ -4789,7 +4798,7 @@
       <c r="E122" s="73"/>
       <c r="F122" s="61"/>
     </row>
-    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="69"/>
       <c r="B123" s="70"/>
       <c r="C123" s="71"/>
@@ -4797,7 +4806,7 @@
       <c r="E123" s="73"/>
       <c r="F123" s="61"/>
     </row>
-    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="69"/>
       <c r="B124" s="70"/>
       <c r="C124" s="71"/>
@@ -4805,7 +4814,7 @@
       <c r="E124" s="73"/>
       <c r="F124" s="61"/>
     </row>
-    <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="69"/>
       <c r="B125" s="70"/>
       <c r="C125" s="71"/>
@@ -4813,7 +4822,7 @@
       <c r="E125" s="73"/>
       <c r="F125" s="61"/>
     </row>
-    <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="69"/>
       <c r="B126" s="70"/>
       <c r="C126" s="71"/>
@@ -4821,7 +4830,7 @@
       <c r="E126" s="73"/>
       <c r="F126" s="61"/>
     </row>
-    <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="69"/>
       <c r="B127" s="70"/>
       <c r="C127" s="71"/>
@@ -4829,7 +4838,7 @@
       <c r="E127" s="73"/>
       <c r="F127" s="61"/>
     </row>
-    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="69"/>
       <c r="B128" s="70"/>
       <c r="C128" s="71"/>
@@ -4837,7 +4846,7 @@
       <c r="E128" s="73"/>
       <c r="F128" s="61"/>
     </row>
-    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="69"/>
       <c r="B129" s="70"/>
       <c r="C129" s="71"/>
@@ -4845,7 +4854,7 @@
       <c r="E129" s="73"/>
       <c r="F129" s="61"/>
     </row>
-    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="69"/>
       <c r="B130" s="70"/>
       <c r="C130" s="71"/>
@@ -4853,7 +4862,7 @@
       <c r="E130" s="73"/>
       <c r="F130" s="61"/>
     </row>
-    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="69"/>
       <c r="B131" s="70"/>
       <c r="C131" s="71"/>
@@ -4861,7 +4870,7 @@
       <c r="E131" s="73"/>
       <c r="F131" s="61"/>
     </row>
-    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="69"/>
       <c r="B132" s="70"/>
       <c r="C132" s="71"/>
@@ -4869,7 +4878,7 @@
       <c r="E132" s="73"/>
       <c r="F132" s="61"/>
     </row>
-    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="69"/>
       <c r="B133" s="70"/>
       <c r="C133" s="71"/>
@@ -4877,7 +4886,7 @@
       <c r="E133" s="73"/>
       <c r="F133" s="61"/>
     </row>
-    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="69"/>
       <c r="B134" s="70"/>
       <c r="C134" s="71"/>
@@ -4885,7 +4894,7 @@
       <c r="E134" s="73"/>
       <c r="F134" s="61"/>
     </row>
-    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="69"/>
       <c r="B135" s="70"/>
       <c r="C135" s="71"/>
@@ -4893,7 +4902,7 @@
       <c r="E135" s="73"/>
       <c r="F135" s="61"/>
     </row>
-    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="69"/>
       <c r="B136" s="70"/>
       <c r="C136" s="71"/>
@@ -4901,7 +4910,7 @@
       <c r="E136" s="73"/>
       <c r="F136" s="61"/>
     </row>
-    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="69"/>
       <c r="B137" s="70"/>
       <c r="C137" s="71"/>
@@ -4909,7 +4918,7 @@
       <c r="E137" s="73"/>
       <c r="F137" s="61"/>
     </row>
-    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="69"/>
       <c r="B138" s="70"/>
       <c r="C138" s="71"/>
@@ -4917,7 +4926,7 @@
       <c r="E138" s="73"/>
       <c r="F138" s="61"/>
     </row>
-    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="69"/>
       <c r="B139" s="70"/>
       <c r="C139" s="71"/>
@@ -4925,7 +4934,7 @@
       <c r="E139" s="73"/>
       <c r="F139" s="61"/>
     </row>
-    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="69"/>
       <c r="B140" s="70"/>
       <c r="C140" s="71"/>
@@ -4933,7 +4942,7 @@
       <c r="E140" s="73"/>
       <c r="F140" s="61"/>
     </row>
-    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="69"/>
       <c r="B141" s="70"/>
       <c r="C141" s="71"/>
@@ -4941,7 +4950,7 @@
       <c r="E141" s="73"/>
       <c r="F141" s="61"/>
     </row>
-    <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="69"/>
       <c r="B142" s="70"/>
       <c r="C142" s="71"/>
@@ -4949,7 +4958,7 @@
       <c r="E142" s="73"/>
       <c r="F142" s="61"/>
     </row>
-    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="69"/>
       <c r="B143" s="70"/>
       <c r="C143" s="71"/>
@@ -4957,7 +4966,7 @@
       <c r="E143" s="73"/>
       <c r="F143" s="61"/>
     </row>
-    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="69"/>
       <c r="B144" s="70"/>
       <c r="C144" s="71"/>
@@ -4965,7 +4974,7 @@
       <c r="E144" s="73"/>
       <c r="F144" s="61"/>
     </row>
-    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="69"/>
       <c r="B145" s="70"/>
       <c r="C145" s="71"/>
@@ -4973,7 +4982,7 @@
       <c r="E145" s="73"/>
       <c r="F145" s="61"/>
     </row>
-    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="69"/>
       <c r="B146" s="70"/>
       <c r="C146" s="71"/>
@@ -4981,7 +4990,7 @@
       <c r="E146" s="73"/>
       <c r="F146" s="61"/>
     </row>
-    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="69"/>
       <c r="B147" s="70"/>
       <c r="C147" s="71"/>
@@ -4989,7 +4998,7 @@
       <c r="E147" s="73"/>
       <c r="F147" s="61"/>
     </row>
-    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="69"/>
       <c r="B148" s="70"/>
       <c r="C148" s="71"/>
@@ -4997,7 +5006,7 @@
       <c r="E148" s="73"/>
       <c r="F148" s="61"/>
     </row>
-    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="69"/>
       <c r="B149" s="70"/>
       <c r="C149" s="71"/>
@@ -5005,7 +5014,7 @@
       <c r="E149" s="73"/>
       <c r="F149" s="61"/>
     </row>
-    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="69"/>
       <c r="B150" s="70"/>
       <c r="C150" s="71"/>
@@ -5013,7 +5022,7 @@
       <c r="E150" s="73"/>
       <c r="F150" s="61"/>
     </row>
-    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="69"/>
       <c r="B151" s="70"/>
       <c r="C151" s="71"/>
@@ -5021,7 +5030,7 @@
       <c r="E151" s="73"/>
       <c r="F151" s="61"/>
     </row>
-    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="69"/>
       <c r="B152" s="70"/>
       <c r="C152" s="71"/>
@@ -5029,7 +5038,7 @@
       <c r="E152" s="73"/>
       <c r="F152" s="61"/>
     </row>
-    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="69"/>
       <c r="B153" s="70"/>
       <c r="C153" s="71"/>
@@ -5037,7 +5046,7 @@
       <c r="E153" s="73"/>
       <c r="F153" s="61"/>
     </row>
-    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="69"/>
       <c r="B154" s="70"/>
       <c r="C154" s="71"/>
@@ -5045,7 +5054,7 @@
       <c r="E154" s="73"/>
       <c r="F154" s="61"/>
     </row>
-    <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="69"/>
       <c r="B155" s="70"/>
       <c r="C155" s="71"/>
@@ -5053,7 +5062,7 @@
       <c r="E155" s="73"/>
       <c r="F155" s="61"/>
     </row>
-    <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="69"/>
       <c r="B156" s="70"/>
       <c r="C156" s="71"/>
@@ -5061,7 +5070,7 @@
       <c r="E156" s="73"/>
       <c r="F156" s="61"/>
     </row>
-    <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="69"/>
       <c r="B157" s="70"/>
       <c r="C157" s="71"/>
@@ -5069,7 +5078,7 @@
       <c r="E157" s="73"/>
       <c r="F157" s="61"/>
     </row>
-    <row r="158" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="69"/>
       <c r="B158" s="70"/>
       <c r="C158" s="71"/>
@@ -5077,7 +5086,7 @@
       <c r="E158" s="73"/>
       <c r="F158" s="61"/>
     </row>
-    <row r="159" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="69"/>
       <c r="B159" s="70"/>
       <c r="C159" s="71"/>
@@ -5085,7 +5094,7 @@
       <c r="E159" s="73"/>
       <c r="F159" s="61"/>
     </row>
-    <row r="160" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="69"/>
       <c r="B160" s="70"/>
       <c r="C160" s="71"/>
@@ -5093,7 +5102,7 @@
       <c r="E160" s="73"/>
       <c r="F160" s="61"/>
     </row>
-    <row r="161" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="69"/>
       <c r="B161" s="70"/>
       <c r="C161" s="71"/>
@@ -5101,7 +5110,7 @@
       <c r="E161" s="73"/>
       <c r="F161" s="61"/>
     </row>
-    <row r="162" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="69"/>
       <c r="B162" s="70"/>
       <c r="C162" s="71"/>
@@ -5109,7 +5118,7 @@
       <c r="E162" s="73"/>
       <c r="F162" s="61"/>
     </row>
-    <row r="163" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="69"/>
       <c r="B163" s="70"/>
       <c r="C163" s="71"/>
@@ -5117,7 +5126,7 @@
       <c r="E163" s="73"/>
       <c r="F163" s="61"/>
     </row>
-    <row r="164" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="69"/>
       <c r="B164" s="70"/>
       <c r="C164" s="71"/>
@@ -5125,7 +5134,7 @@
       <c r="E164" s="73"/>
       <c r="F164" s="61"/>
     </row>
-    <row r="165" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="69"/>
       <c r="B165" s="70"/>
       <c r="C165" s="71"/>
@@ -5133,7 +5142,7 @@
       <c r="E165" s="73"/>
       <c r="F165" s="61"/>
     </row>
-    <row r="166" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="69"/>
       <c r="B166" s="70"/>
       <c r="C166" s="71"/>
@@ -5141,7 +5150,7 @@
       <c r="E166" s="73"/>
       <c r="F166" s="61"/>
     </row>
-    <row r="167" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="69"/>
       <c r="B167" s="70"/>
       <c r="C167" s="71"/>
@@ -5149,7 +5158,7 @@
       <c r="E167" s="73"/>
       <c r="F167" s="61"/>
     </row>
-    <row r="168" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="69"/>
       <c r="B168" s="70"/>
       <c r="C168" s="71"/>
@@ -5157,7 +5166,7 @@
       <c r="E168" s="73"/>
       <c r="F168" s="61"/>
     </row>
-    <row r="169" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="69"/>
       <c r="B169" s="70"/>
       <c r="C169" s="71"/>
@@ -5165,7 +5174,7 @@
       <c r="E169" s="73"/>
       <c r="F169" s="61"/>
     </row>
-    <row r="170" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="69"/>
       <c r="B170" s="70"/>
       <c r="C170" s="71"/>
@@ -5173,7 +5182,7 @@
       <c r="E170" s="73"/>
       <c r="F170" s="61"/>
     </row>
-    <row r="171" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="69"/>
       <c r="B171" s="70"/>
       <c r="C171" s="71"/>
@@ -5181,7 +5190,7 @@
       <c r="E171" s="73"/>
       <c r="F171" s="61"/>
     </row>
-    <row r="172" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="69"/>
       <c r="B172" s="70"/>
       <c r="C172" s="71"/>
@@ -5189,7 +5198,7 @@
       <c r="E172" s="73"/>
       <c r="F172" s="61"/>
     </row>
-    <row r="173" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="69"/>
       <c r="B173" s="70"/>
       <c r="C173" s="71"/>
@@ -5197,7 +5206,7 @@
       <c r="E173" s="73"/>
       <c r="F173" s="61"/>
     </row>
-    <row r="174" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="69"/>
       <c r="B174" s="70"/>
       <c r="C174" s="71"/>
@@ -5205,7 +5214,7 @@
       <c r="E174" s="73"/>
       <c r="F174" s="61"/>
     </row>
-    <row r="175" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="69"/>
       <c r="B175" s="70"/>
       <c r="C175" s="71"/>
@@ -5213,7 +5222,7 @@
       <c r="E175" s="73"/>
       <c r="F175" s="61"/>
     </row>
-    <row r="176" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="69"/>
       <c r="B176" s="70"/>
       <c r="C176" s="71"/>
@@ -5221,7 +5230,7 @@
       <c r="E176" s="73"/>
       <c r="F176" s="61"/>
     </row>
-    <row r="177" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A177" s="69"/>
       <c r="B177" s="70"/>
       <c r="C177" s="71"/>
@@ -5229,7 +5238,7 @@
       <c r="E177" s="73"/>
       <c r="F177" s="61"/>
     </row>
-    <row r="178" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="69"/>
       <c r="B178" s="70"/>
       <c r="C178" s="71"/>
@@ -5237,7 +5246,7 @@
       <c r="E178" s="73"/>
       <c r="F178" s="61"/>
     </row>
-    <row r="179" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" s="69"/>
       <c r="B179" s="70"/>
       <c r="C179" s="71"/>
@@ -5245,7 +5254,7 @@
       <c r="E179" s="73"/>
       <c r="F179" s="61"/>
     </row>
-    <row r="180" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A180" s="69"/>
       <c r="B180" s="70"/>
       <c r="C180" s="71"/>
@@ -5253,7 +5262,7 @@
       <c r="E180" s="73"/>
       <c r="F180" s="61"/>
     </row>
-    <row r="181" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A181" s="69"/>
       <c r="B181" s="70"/>
       <c r="C181" s="71"/>
@@ -5261,7 +5270,7 @@
       <c r="E181" s="73"/>
       <c r="F181" s="61"/>
     </row>
-    <row r="182" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A182" s="69"/>
       <c r="B182" s="70"/>
       <c r="C182" s="71"/>
@@ -5269,7 +5278,7 @@
       <c r="E182" s="73"/>
       <c r="F182" s="61"/>
     </row>
-    <row r="183" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A183" s="69"/>
       <c r="B183" s="70"/>
       <c r="C183" s="71"/>
@@ -5277,7 +5286,7 @@
       <c r="E183" s="73"/>
       <c r="F183" s="61"/>
     </row>
-    <row r="184" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="69"/>
       <c r="B184" s="70"/>
       <c r="C184" s="71"/>
@@ -5285,7 +5294,7 @@
       <c r="E184" s="73"/>
       <c r="F184" s="61"/>
     </row>
-    <row r="185" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" s="69"/>
       <c r="B185" s="70"/>
       <c r="C185" s="71"/>
@@ -5293,7 +5302,7 @@
       <c r="E185" s="73"/>
       <c r="F185" s="61"/>
     </row>
-    <row r="186" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="69"/>
       <c r="B186" s="70"/>
       <c r="C186" s="71"/>
@@ -5301,7 +5310,7 @@
       <c r="E186" s="73"/>
       <c r="F186" s="61"/>
     </row>
-    <row r="187" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="69"/>
       <c r="B187" s="70"/>
       <c r="C187" s="71"/>
@@ -5309,7 +5318,7 @@
       <c r="E187" s="73"/>
       <c r="F187" s="61"/>
     </row>
-    <row r="188" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A188" s="69"/>
       <c r="B188" s="70"/>
       <c r="C188" s="71"/>
@@ -5317,7 +5326,7 @@
       <c r="E188" s="73"/>
       <c r="F188" s="61"/>
     </row>
-    <row r="189" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="69"/>
       <c r="B189" s="70"/>
       <c r="C189" s="71"/>
@@ -5325,7 +5334,7 @@
       <c r="E189" s="73"/>
       <c r="F189" s="61"/>
     </row>
-    <row r="190" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="69"/>
       <c r="B190" s="70"/>
       <c r="C190" s="71"/>
@@ -5333,7 +5342,7 @@
       <c r="E190" s="73"/>
       <c r="F190" s="61"/>
     </row>
-    <row r="191" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A191" s="69"/>
       <c r="B191" s="70"/>
       <c r="C191" s="71"/>
@@ -5341,7 +5350,7 @@
       <c r="E191" s="73"/>
       <c r="F191" s="61"/>
     </row>
-    <row r="192" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A192" s="69"/>
       <c r="B192" s="70"/>
       <c r="C192" s="71"/>
@@ -5349,7 +5358,7 @@
       <c r="E192" s="73"/>
       <c r="F192" s="61"/>
     </row>
-    <row r="193" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="69"/>
       <c r="B193" s="70"/>
       <c r="C193" s="71"/>
@@ -5357,7 +5366,7 @@
       <c r="E193" s="73"/>
       <c r="F193" s="61"/>
     </row>
-    <row r="194" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A194" s="69"/>
       <c r="B194" s="70"/>
       <c r="C194" s="71"/>
@@ -5365,7 +5374,7 @@
       <c r="E194" s="73"/>
       <c r="F194" s="61"/>
     </row>
-    <row r="195" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A195" s="69"/>
       <c r="B195" s="70"/>
       <c r="C195" s="71"/>
@@ -5373,7 +5382,7 @@
       <c r="E195" s="73"/>
       <c r="F195" s="61"/>
     </row>
-    <row r="196" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A196" s="69"/>
       <c r="B196" s="70"/>
       <c r="C196" s="71"/>
@@ -5381,7 +5390,7 @@
       <c r="E196" s="73"/>
       <c r="F196" s="61"/>
     </row>
-    <row r="197" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="69"/>
       <c r="B197" s="70"/>
       <c r="C197" s="71"/>
@@ -5389,7 +5398,7 @@
       <c r="E197" s="73"/>
       <c r="F197" s="61"/>
     </row>
-    <row r="198" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A198" s="69"/>
       <c r="B198" s="70"/>
       <c r="C198" s="71"/>
@@ -5397,7 +5406,7 @@
       <c r="E198" s="73"/>
       <c r="F198" s="61"/>
     </row>
-    <row r="199" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="69"/>
       <c r="B199" s="70"/>
       <c r="C199" s="71"/>
@@ -5405,7 +5414,7 @@
       <c r="E199" s="73"/>
       <c r="F199" s="61"/>
     </row>
-    <row r="200" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="69"/>
       <c r="B200" s="70"/>
       <c r="C200" s="71"/>
@@ -5413,7 +5422,7 @@
       <c r="E200" s="73"/>
       <c r="F200" s="61"/>
     </row>
-    <row r="201" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="69"/>
       <c r="B201" s="70"/>
       <c r="C201" s="71"/>
@@ -5421,7 +5430,7 @@
       <c r="E201" s="73"/>
       <c r="F201" s="61"/>
     </row>
-    <row r="202" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="69"/>
       <c r="B202" s="70"/>
       <c r="C202" s="71"/>
@@ -5429,7 +5438,7 @@
       <c r="E202" s="73"/>
       <c r="F202" s="61"/>
     </row>
-    <row r="203" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="69"/>
       <c r="B203" s="70"/>
       <c r="C203" s="71"/>
@@ -5437,7 +5446,7 @@
       <c r="E203" s="73"/>
       <c r="F203" s="61"/>
     </row>
-    <row r="204" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="69"/>
       <c r="B204" s="70"/>
       <c r="C204" s="71"/>
@@ -5445,7 +5454,7 @@
       <c r="E204" s="73"/>
       <c r="F204" s="61"/>
     </row>
-    <row r="205" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="69"/>
       <c r="B205" s="70"/>
       <c r="C205" s="71"/>
@@ -5453,7 +5462,7 @@
       <c r="E205" s="73"/>
       <c r="F205" s="61"/>
     </row>
-    <row r="206" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="69"/>
       <c r="B206" s="70"/>
       <c r="C206" s="71"/>
@@ -5461,7 +5470,7 @@
       <c r="E206" s="73"/>
       <c r="F206" s="61"/>
     </row>
-    <row r="207" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="69"/>
       <c r="B207" s="70"/>
       <c r="C207" s="71"/>
@@ -5469,7 +5478,7 @@
       <c r="E207" s="73"/>
       <c r="F207" s="61"/>
     </row>
-    <row r="208" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="69"/>
       <c r="B208" s="70"/>
       <c r="C208" s="71"/>
@@ -5477,7 +5486,7 @@
       <c r="E208" s="73"/>
       <c r="F208" s="61"/>
     </row>
-    <row r="209" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="69"/>
       <c r="B209" s="70"/>
       <c r="C209" s="71"/>
@@ -5485,7 +5494,7 @@
       <c r="E209" s="73"/>
       <c r="F209" s="61"/>
     </row>
-    <row r="210" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="69"/>
       <c r="B210" s="70"/>
       <c r="C210" s="71"/>
@@ -5493,7 +5502,7 @@
       <c r="E210" s="73"/>
       <c r="F210" s="61"/>
     </row>
-    <row r="211" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A211" s="69"/>
       <c r="B211" s="70"/>
       <c r="C211" s="71"/>
@@ -5501,7 +5510,7 @@
       <c r="E211" s="73"/>
       <c r="F211" s="61"/>
     </row>
-    <row r="212" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="69"/>
       <c r="B212" s="70"/>
       <c r="C212" s="71"/>
@@ -5509,7 +5518,7 @@
       <c r="E212" s="73"/>
       <c r="F212" s="61"/>
     </row>
-    <row r="213" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="69"/>
       <c r="B213" s="70"/>
       <c r="C213" s="71"/>
@@ -5517,7 +5526,7 @@
       <c r="E213" s="73"/>
       <c r="F213" s="61"/>
     </row>
-    <row r="214" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="69"/>
       <c r="B214" s="70"/>
       <c r="C214" s="71"/>
@@ -5525,7 +5534,7 @@
       <c r="E214" s="73"/>
       <c r="F214" s="61"/>
     </row>
-    <row r="215" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A215" s="69"/>
       <c r="B215" s="70"/>
       <c r="C215" s="71"/>
@@ -5533,7 +5542,7 @@
       <c r="E215" s="73"/>
       <c r="F215" s="61"/>
     </row>
-    <row r="216" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="69"/>
       <c r="B216" s="70"/>
       <c r="C216" s="71"/>
@@ -5541,7 +5550,7 @@
       <c r="E216" s="73"/>
       <c r="F216" s="61"/>
     </row>
-    <row r="217" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A217" s="69"/>
       <c r="B217" s="70"/>
       <c r="C217" s="71"/>
@@ -5549,7 +5558,7 @@
       <c r="E217" s="73"/>
       <c r="F217" s="61"/>
     </row>
-    <row r="218" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A218" s="69"/>
       <c r="B218" s="70"/>
       <c r="C218" s="71"/>
@@ -5557,7 +5566,7 @@
       <c r="E218" s="73"/>
       <c r="F218" s="61"/>
     </row>
-    <row r="219" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A219" s="69"/>
       <c r="B219" s="70"/>
       <c r="C219" s="71"/>
@@ -5565,7 +5574,7 @@
       <c r="E219" s="73"/>
       <c r="F219" s="61"/>
     </row>
-    <row r="220" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="69"/>
       <c r="B220" s="70"/>
       <c r="C220" s="71"/>
@@ -5573,7 +5582,7 @@
       <c r="E220" s="73"/>
       <c r="F220" s="61"/>
     </row>
-    <row r="221" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="69"/>
       <c r="B221" s="70"/>
       <c r="C221" s="71"/>
@@ -5581,7 +5590,7 @@
       <c r="E221" s="73"/>
       <c r="F221" s="61"/>
     </row>
-    <row r="222" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="69"/>
       <c r="B222" s="70"/>
       <c r="C222" s="71"/>
@@ -5589,7 +5598,7 @@
       <c r="E222" s="73"/>
       <c r="F222" s="61"/>
     </row>
-    <row r="223" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="69"/>
       <c r="B223" s="70"/>
       <c r="C223" s="71"/>
@@ -5597,7 +5606,7 @@
       <c r="E223" s="73"/>
       <c r="F223" s="61"/>
     </row>
-    <row r="224" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="69"/>
       <c r="B224" s="70"/>
       <c r="C224" s="71"/>
@@ -5605,7 +5614,7 @@
       <c r="E224" s="73"/>
       <c r="F224" s="61"/>
     </row>
-    <row r="225" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A225" s="69"/>
       <c r="B225" s="70"/>
       <c r="C225" s="71"/>
@@ -5613,7 +5622,7 @@
       <c r="E225" s="73"/>
       <c r="F225" s="61"/>
     </row>
-    <row r="226" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" s="69"/>
       <c r="B226" s="70"/>
       <c r="C226" s="71"/>
@@ -5621,7 +5630,7 @@
       <c r="E226" s="73"/>
       <c r="F226" s="61"/>
     </row>
-    <row r="227" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="69"/>
       <c r="B227" s="70"/>
       <c r="C227" s="71"/>
@@ -5629,7 +5638,7 @@
       <c r="E227" s="73"/>
       <c r="F227" s="61"/>
     </row>
-    <row r="228" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A228" s="69"/>
       <c r="B228" s="70"/>
       <c r="C228" s="71"/>
@@ -5637,7 +5646,7 @@
       <c r="E228" s="73"/>
       <c r="F228" s="61"/>
     </row>
-    <row r="229" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" s="69"/>
       <c r="B229" s="70"/>
       <c r="C229" s="71"/>
@@ -5645,7 +5654,7 @@
       <c r="E229" s="73"/>
       <c r="F229" s="61"/>
     </row>
-    <row r="230" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A230" s="69"/>
       <c r="B230" s="70"/>
       <c r="C230" s="71"/>
@@ -5653,7 +5662,7 @@
       <c r="E230" s="73"/>
       <c r="F230" s="61"/>
     </row>
-    <row r="231" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A231" s="69"/>
       <c r="B231" s="70"/>
       <c r="C231" s="71"/>
@@ -5661,7 +5670,7 @@
       <c r="E231" s="73"/>
       <c r="F231" s="61"/>
     </row>
-    <row r="232" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A232" s="69"/>
       <c r="B232" s="70"/>
       <c r="C232" s="71"/>
@@ -5669,7 +5678,7 @@
       <c r="E232" s="73"/>
       <c r="F232" s="61"/>
     </row>
-    <row r="233" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A233" s="69"/>
       <c r="B233" s="70"/>
       <c r="C233" s="71"/>
@@ -5677,7 +5686,7 @@
       <c r="E233" s="73"/>
       <c r="F233" s="61"/>
     </row>
-    <row r="234" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" s="69"/>
       <c r="B234" s="70"/>
       <c r="C234" s="71"/>
@@ -5685,7 +5694,7 @@
       <c r="E234" s="73"/>
       <c r="F234" s="61"/>
     </row>
-    <row r="235" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A235" s="69"/>
       <c r="B235" s="70"/>
       <c r="C235" s="71"/>
@@ -5693,7 +5702,7 @@
       <c r="E235" s="73"/>
       <c r="F235" s="61"/>
     </row>
-    <row r="236" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A236" s="69"/>
       <c r="B236" s="70"/>
       <c r="C236" s="71"/>
@@ -5701,7 +5710,7 @@
       <c r="E236" s="73"/>
       <c r="F236" s="61"/>
     </row>
-    <row r="237" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A237" s="69"/>
       <c r="B237" s="70"/>
       <c r="C237" s="71"/>
@@ -5709,7 +5718,7 @@
       <c r="E237" s="73"/>
       <c r="F237" s="61"/>
     </row>
-    <row r="238" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A238" s="69"/>
       <c r="B238" s="70"/>
       <c r="C238" s="71"/>
@@ -5717,7 +5726,7 @@
       <c r="E238" s="73"/>
       <c r="F238" s="61"/>
     </row>
-    <row r="239" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A239" s="69"/>
       <c r="B239" s="70"/>
       <c r="C239" s="71"/>
@@ -5725,7 +5734,7 @@
       <c r="E239" s="73"/>
       <c r="F239" s="61"/>
     </row>
-    <row r="240" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A240" s="69"/>
       <c r="B240" s="70"/>
       <c r="C240" s="71"/>
@@ -5733,7 +5742,7 @@
       <c r="E240" s="73"/>
       <c r="F240" s="61"/>
     </row>
-    <row r="241" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A241" s="69"/>
       <c r="B241" s="70"/>
       <c r="C241" s="71"/>
@@ -5741,7 +5750,7 @@
       <c r="E241" s="73"/>
       <c r="F241" s="61"/>
     </row>
-    <row r="242" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A242" s="69"/>
       <c r="B242" s="70"/>
       <c r="C242" s="71"/>
@@ -5749,7 +5758,7 @@
       <c r="E242" s="73"/>
       <c r="F242" s="61"/>
     </row>
-    <row r="243" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A243" s="69"/>
       <c r="B243" s="70"/>
       <c r="C243" s="71"/>
@@ -5757,7 +5766,7 @@
       <c r="E243" s="73"/>
       <c r="F243" s="61"/>
     </row>
-    <row r="244" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A244" s="69"/>
       <c r="B244" s="70"/>
       <c r="C244" s="71"/>
@@ -5765,7 +5774,7 @@
       <c r="E244" s="73"/>
       <c r="F244" s="61"/>
     </row>
-    <row r="245" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A245" s="69"/>
       <c r="B245" s="70"/>
       <c r="C245" s="71"/>
@@ -5773,7 +5782,7 @@
       <c r="E245" s="73"/>
       <c r="F245" s="61"/>
     </row>
-    <row r="246" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A246" s="69"/>
       <c r="B246" s="70"/>
       <c r="C246" s="71"/>
@@ -5781,7 +5790,7 @@
       <c r="E246" s="73"/>
       <c r="F246" s="61"/>
     </row>
-    <row r="247" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A247" s="69"/>
       <c r="B247" s="70"/>
       <c r="C247" s="71"/>
@@ -5789,7 +5798,7 @@
       <c r="E247" s="73"/>
       <c r="F247" s="61"/>
     </row>
-    <row r="248" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A248" s="69"/>
       <c r="B248" s="70"/>
       <c r="C248" s="71"/>
@@ -5797,7 +5806,7 @@
       <c r="E248" s="73"/>
       <c r="F248" s="61"/>
     </row>
-    <row r="249" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A249" s="69"/>
       <c r="B249" s="70"/>
       <c r="C249" s="71"/>
@@ -5805,7 +5814,7 @@
       <c r="E249" s="73"/>
       <c r="F249" s="61"/>
     </row>
-    <row r="250" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A250" s="69"/>
       <c r="B250" s="70"/>
       <c r="C250" s="71"/>
@@ -5813,7 +5822,7 @@
       <c r="E250" s="73"/>
       <c r="F250" s="61"/>
     </row>
-    <row r="251" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A251" s="69"/>
       <c r="B251" s="70"/>
       <c r="C251" s="71"/>
@@ -5821,7 +5830,7 @@
       <c r="E251" s="73"/>
       <c r="F251" s="61"/>
     </row>
-    <row r="252" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A252" s="69"/>
       <c r="B252" s="70"/>
       <c r="C252" s="71"/>
@@ -5829,7 +5838,7 @@
       <c r="E252" s="73"/>
       <c r="F252" s="61"/>
     </row>
-    <row r="253" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A253" s="69"/>
       <c r="B253" s="70"/>
       <c r="C253" s="71"/>
@@ -5837,7 +5846,7 @@
       <c r="E253" s="73"/>
       <c r="F253" s="61"/>
     </row>
-    <row r="254" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A254" s="69"/>
       <c r="B254" s="70"/>
       <c r="C254" s="71"/>
@@ -5845,7 +5854,7 @@
       <c r="E254" s="73"/>
       <c r="F254" s="61"/>
     </row>
-    <row r="255" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A255" s="69"/>
       <c r="B255" s="70"/>
       <c r="C255" s="71"/>
@@ -5853,7 +5862,7 @@
       <c r="E255" s="73"/>
       <c r="F255" s="61"/>
     </row>
-    <row r="256" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A256" s="69"/>
       <c r="B256" s="70"/>
       <c r="C256" s="71"/>
@@ -5861,7 +5870,7 @@
       <c r="E256" s="73"/>
       <c r="F256" s="61"/>
     </row>
-    <row r="257" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A257" s="69"/>
       <c r="B257" s="70"/>
       <c r="C257" s="71"/>
@@ -5869,7 +5878,7 @@
       <c r="E257" s="73"/>
       <c r="F257" s="61"/>
     </row>
-    <row r="258" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A258" s="69"/>
       <c r="B258" s="70"/>
       <c r="C258" s="71"/>
@@ -5877,7 +5886,7 @@
       <c r="E258" s="73"/>
       <c r="F258" s="61"/>
     </row>
-    <row r="259" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A259" s="69"/>
       <c r="B259" s="70"/>
       <c r="C259" s="71"/>
@@ -5885,7 +5894,7 @@
       <c r="E259" s="73"/>
       <c r="F259" s="61"/>
     </row>
-    <row r="260" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A260" s="69"/>
       <c r="B260" s="70"/>
       <c r="C260" s="71"/>
@@ -5893,7 +5902,7 @@
       <c r="E260" s="73"/>
       <c r="F260" s="61"/>
     </row>
-    <row r="261" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A261" s="69"/>
       <c r="B261" s="70"/>
       <c r="C261" s="71"/>
@@ -5901,7 +5910,7 @@
       <c r="E261" s="73"/>
       <c r="F261" s="61"/>
     </row>
-    <row r="262" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A262" s="69"/>
       <c r="B262" s="70"/>
       <c r="C262" s="71"/>
@@ -5909,7 +5918,7 @@
       <c r="E262" s="73"/>
       <c r="F262" s="61"/>
     </row>
-    <row r="263" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A263" s="69"/>
       <c r="B263" s="70"/>
       <c r="C263" s="71"/>
@@ -5917,7 +5926,7 @@
       <c r="E263" s="73"/>
       <c r="F263" s="61"/>
     </row>
-    <row r="264" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A264" s="69"/>
       <c r="B264" s="70"/>
       <c r="C264" s="71"/>
@@ -5925,7 +5934,7 @@
       <c r="E264" s="73"/>
       <c r="F264" s="61"/>
     </row>
-    <row r="265" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A265" s="69"/>
       <c r="B265" s="70"/>
       <c r="C265" s="71"/>
@@ -5933,7 +5942,7 @@
       <c r="E265" s="73"/>
       <c r="F265" s="61"/>
     </row>
-    <row r="266" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A266" s="69"/>
       <c r="B266" s="70"/>
       <c r="C266" s="71"/>
@@ -5941,7 +5950,7 @@
       <c r="E266" s="73"/>
       <c r="F266" s="61"/>
     </row>
-    <row r="267" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A267" s="69"/>
       <c r="B267" s="70"/>
       <c r="C267" s="71"/>
@@ -5949,7 +5958,7 @@
       <c r="E267" s="73"/>
       <c r="F267" s="61"/>
     </row>
-    <row r="268" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A268" s="69"/>
       <c r="B268" s="70"/>
       <c r="C268" s="71"/>
@@ -5957,7 +5966,7 @@
       <c r="E268" s="73"/>
       <c r="F268" s="61"/>
     </row>
-    <row r="269" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A269" s="69"/>
       <c r="B269" s="70"/>
       <c r="C269" s="71"/>
@@ -5965,7 +5974,7 @@
       <c r="E269" s="73"/>
       <c r="F269" s="61"/>
     </row>
-    <row r="270" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A270" s="69"/>
       <c r="B270" s="70"/>
       <c r="C270" s="71"/>
@@ -5973,7 +5982,7 @@
       <c r="E270" s="73"/>
       <c r="F270" s="61"/>
     </row>
-    <row r="271" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A271" s="69"/>
       <c r="B271" s="70"/>
       <c r="C271" s="71"/>
@@ -5981,7 +5990,7 @@
       <c r="E271" s="73"/>
       <c r="F271" s="61"/>
     </row>
-    <row r="272" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A272" s="69"/>
       <c r="B272" s="70"/>
       <c r="C272" s="71"/>
@@ -5989,7 +5998,7 @@
       <c r="E272" s="73"/>
       <c r="F272" s="61"/>
     </row>
-    <row r="273" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A273" s="69"/>
       <c r="B273" s="70"/>
       <c r="C273" s="71"/>
@@ -5997,7 +6006,7 @@
       <c r="E273" s="73"/>
       <c r="F273" s="61"/>
     </row>
-    <row r="274" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A274" s="69"/>
       <c r="B274" s="70"/>
       <c r="C274" s="71"/>
@@ -6005,7 +6014,7 @@
       <c r="E274" s="73"/>
       <c r="F274" s="61"/>
     </row>
-    <row r="275" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A275" s="69"/>
       <c r="B275" s="70"/>
       <c r="C275" s="71"/>
@@ -6013,7 +6022,7 @@
       <c r="E275" s="73"/>
       <c r="F275" s="61"/>
     </row>
-    <row r="276" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A276" s="69"/>
       <c r="B276" s="70"/>
       <c r="C276" s="71"/>
@@ -6021,7 +6030,7 @@
       <c r="E276" s="73"/>
       <c r="F276" s="61"/>
     </row>
-    <row r="277" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A277" s="69"/>
       <c r="B277" s="70"/>
       <c r="C277" s="71"/>
@@ -6029,7 +6038,7 @@
       <c r="E277" s="73"/>
       <c r="F277" s="61"/>
     </row>
-    <row r="278" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A278" s="69"/>
       <c r="B278" s="70"/>
       <c r="C278" s="71"/>
@@ -6037,7 +6046,7 @@
       <c r="E278" s="73"/>
       <c r="F278" s="61"/>
     </row>
-    <row r="279" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A279" s="69"/>
       <c r="B279" s="70"/>
       <c r="C279" s="71"/>
@@ -6045,7 +6054,7 @@
       <c r="E279" s="73"/>
       <c r="F279" s="61"/>
     </row>
-    <row r="280" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A280" s="69"/>
       <c r="B280" s="70"/>
       <c r="C280" s="71"/>
@@ -6053,7 +6062,7 @@
       <c r="E280" s="73"/>
       <c r="F280" s="61"/>
     </row>
-    <row r="281" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A281" s="69"/>
       <c r="B281" s="70"/>
       <c r="C281" s="71"/>
@@ -6061,7 +6070,7 @@
       <c r="E281" s="73"/>
       <c r="F281" s="61"/>
     </row>
-    <row r="282" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A282" s="69"/>
       <c r="B282" s="70"/>
       <c r="C282" s="71"/>
@@ -6069,7 +6078,7 @@
       <c r="E282" s="73"/>
       <c r="F282" s="61"/>
     </row>
-    <row r="283" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A283" s="69"/>
       <c r="B283" s="70"/>
       <c r="C283" s="71"/>
@@ -6077,7 +6086,7 @@
       <c r="E283" s="73"/>
       <c r="F283" s="61"/>
     </row>
-    <row r="284" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A284" s="69"/>
       <c r="B284" s="70"/>
       <c r="C284" s="71"/>
@@ -6085,7 +6094,7 @@
       <c r="E284" s="73"/>
       <c r="F284" s="61"/>
     </row>
-    <row r="285" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A285" s="69"/>
       <c r="B285" s="70"/>
       <c r="C285" s="71"/>
@@ -6093,7 +6102,7 @@
       <c r="E285" s="73"/>
       <c r="F285" s="61"/>
     </row>
-    <row r="286" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A286" s="69"/>
       <c r="B286" s="70"/>
       <c r="C286" s="71"/>
@@ -6101,7 +6110,7 @@
       <c r="E286" s="73"/>
       <c r="F286" s="61"/>
     </row>
-    <row r="287" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A287" s="69"/>
       <c r="B287" s="70"/>
       <c r="C287" s="71"/>
@@ -6109,7 +6118,7 @@
       <c r="E287" s="73"/>
       <c r="F287" s="61"/>
     </row>
-    <row r="288" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A288" s="69"/>
       <c r="B288" s="70"/>
       <c r="C288" s="71"/>
@@ -6117,7 +6126,7 @@
       <c r="E288" s="73"/>
       <c r="F288" s="61"/>
     </row>
-    <row r="289" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A289" s="69"/>
       <c r="B289" s="70"/>
       <c r="C289" s="71"/>
@@ -6125,7 +6134,7 @@
       <c r="E289" s="73"/>
       <c r="F289" s="61"/>
     </row>
-    <row r="290" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A290" s="69"/>
       <c r="B290" s="70"/>
       <c r="C290" s="71"/>
@@ -6133,7 +6142,7 @@
       <c r="E290" s="73"/>
       <c r="F290" s="61"/>
     </row>
-    <row r="291" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A291" s="69"/>
       <c r="B291" s="70"/>
       <c r="C291" s="71"/>
@@ -6141,7 +6150,7 @@
       <c r="E291" s="73"/>
       <c r="F291" s="61"/>
     </row>
-    <row r="292" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A292" s="69"/>
       <c r="B292" s="70"/>
       <c r="C292" s="71"/>
@@ -6149,7 +6158,7 @@
       <c r="E292" s="73"/>
       <c r="F292" s="61"/>
     </row>
-    <row r="293" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A293" s="69"/>
       <c r="B293" s="70"/>
       <c r="C293" s="71"/>
@@ -6157,7 +6166,7 @@
       <c r="E293" s="73"/>
       <c r="F293" s="61"/>
     </row>
-    <row r="294" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A294" s="69"/>
       <c r="B294" s="70"/>
       <c r="C294" s="71"/>
@@ -6165,7 +6174,7 @@
       <c r="E294" s="73"/>
       <c r="F294" s="61"/>
     </row>
-    <row r="295" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A295" s="69"/>
       <c r="B295" s="70"/>
       <c r="C295" s="71"/>
@@ -6173,7 +6182,7 @@
       <c r="E295" s="73"/>
       <c r="F295" s="61"/>
     </row>
-    <row r="296" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A296" s="69"/>
       <c r="B296" s="70"/>
       <c r="C296" s="71"/>
@@ -6181,7 +6190,7 @@
       <c r="E296" s="73"/>
       <c r="F296" s="61"/>
     </row>
-    <row r="297" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A297" s="69"/>
       <c r="B297" s="70"/>
       <c r="C297" s="71"/>
@@ -6189,7 +6198,7 @@
       <c r="E297" s="73"/>
       <c r="F297" s="61"/>
     </row>
-    <row r="298" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A298" s="69"/>
       <c r="B298" s="70"/>
       <c r="C298" s="71"/>
@@ -6197,7 +6206,7 @@
       <c r="E298" s="73"/>
       <c r="F298" s="61"/>
     </row>
-    <row r="299" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A299" s="69"/>
       <c r="B299" s="70"/>
       <c r="C299" s="71"/>
@@ -6205,7 +6214,7 @@
       <c r="E299" s="73"/>
       <c r="F299" s="61"/>
     </row>
-    <row r="300" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A300" s="69"/>
       <c r="B300" s="70"/>
       <c r="C300" s="71"/>
@@ -6213,7 +6222,7 @@
       <c r="E300" s="73"/>
       <c r="F300" s="61"/>
     </row>
-    <row r="301" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A301" s="69"/>
       <c r="B301" s="70"/>
       <c r="C301" s="71"/>
@@ -6221,7 +6230,7 @@
       <c r="E301" s="73"/>
       <c r="F301" s="61"/>
     </row>
-    <row r="302" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A302" s="69"/>
       <c r="B302" s="70"/>
       <c r="C302" s="71"/>
@@ -6229,7 +6238,7 @@
       <c r="E302" s="73"/>
       <c r="F302" s="61"/>
     </row>
-    <row r="303" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A303" s="69"/>
       <c r="B303" s="70"/>
       <c r="C303" s="71"/>
@@ -6237,7 +6246,7 @@
       <c r="E303" s="73"/>
       <c r="F303" s="61"/>
     </row>
-    <row r="304" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A304" s="69"/>
       <c r="B304" s="70"/>
       <c r="C304" s="71"/>
@@ -6245,7 +6254,7 @@
       <c r="E304" s="73"/>
       <c r="F304" s="61"/>
     </row>
-    <row r="305" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A305" s="69"/>
       <c r="B305" s="70"/>
       <c r="C305" s="71"/>
@@ -6253,7 +6262,7 @@
       <c r="E305" s="73"/>
       <c r="F305" s="61"/>
     </row>
-    <row r="306" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A306" s="69"/>
       <c r="B306" s="70"/>
       <c r="C306" s="71"/>
@@ -6261,7 +6270,7 @@
       <c r="E306" s="73"/>
       <c r="F306" s="61"/>
     </row>
-    <row r="307" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A307" s="69"/>
       <c r="B307" s="70"/>
       <c r="C307" s="71"/>
@@ -6269,7 +6278,7 @@
       <c r="E307" s="73"/>
       <c r="F307" s="61"/>
     </row>
-    <row r="308" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A308" s="69"/>
       <c r="B308" s="70"/>
       <c r="C308" s="71"/>
@@ -6277,7 +6286,7 @@
       <c r="E308" s="73"/>
       <c r="F308" s="61"/>
     </row>
-    <row r="309" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A309" s="69"/>
       <c r="B309" s="70"/>
       <c r="C309" s="71"/>
@@ -6285,7 +6294,7 @@
       <c r="E309" s="73"/>
       <c r="F309" s="61"/>
     </row>
-    <row r="310" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A310" s="69"/>
       <c r="B310" s="70"/>
       <c r="C310" s="71"/>
@@ -6293,7 +6302,7 @@
       <c r="E310" s="73"/>
       <c r="F310" s="61"/>
     </row>
-    <row r="311" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A311" s="69"/>
       <c r="B311" s="70"/>
       <c r="C311" s="71"/>
@@ -6301,7 +6310,7 @@
       <c r="E311" s="73"/>
       <c r="F311" s="61"/>
     </row>
-    <row r="312" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A312" s="69"/>
       <c r="B312" s="70"/>
       <c r="C312" s="71"/>
@@ -6309,7 +6318,7 @@
       <c r="E312" s="73"/>
       <c r="F312" s="61"/>
     </row>
-    <row r="313" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A313" s="69"/>
       <c r="B313" s="70"/>
       <c r="C313" s="71"/>
@@ -6317,7 +6326,7 @@
       <c r="E313" s="73"/>
       <c r="F313" s="61"/>
     </row>
-    <row r="314" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A314" s="69"/>
       <c r="B314" s="70"/>
       <c r="C314" s="71"/>
@@ -6325,7 +6334,7 @@
       <c r="E314" s="73"/>
       <c r="F314" s="61"/>
     </row>
-    <row r="315" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A315" s="69"/>
       <c r="B315" s="70"/>
       <c r="C315" s="71"/>
@@ -6333,7 +6342,7 @@
       <c r="E315" s="73"/>
       <c r="F315" s="61"/>
     </row>
-    <row r="316" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A316" s="69"/>
       <c r="B316" s="70"/>
       <c r="C316" s="71"/>
@@ -6341,7 +6350,7 @@
       <c r="E316" s="73"/>
       <c r="F316" s="61"/>
     </row>
-    <row r="317" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A317" s="69"/>
       <c r="B317" s="70"/>
       <c r="C317" s="71"/>
@@ -6349,7 +6358,7 @@
       <c r="E317" s="73"/>
       <c r="F317" s="61"/>
     </row>
-    <row r="318" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A318" s="69"/>
       <c r="B318" s="70"/>
       <c r="C318" s="71"/>
@@ -6357,7 +6366,7 @@
       <c r="E318" s="73"/>
       <c r="F318" s="61"/>
     </row>
-    <row r="319" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A319" s="69"/>
       <c r="B319" s="70"/>
       <c r="C319" s="71"/>
@@ -6365,7 +6374,7 @@
       <c r="E319" s="73"/>
       <c r="F319" s="61"/>
     </row>
-    <row r="320" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A320" s="69"/>
       <c r="B320" s="70"/>
       <c r="C320" s="71"/>
@@ -6373,7 +6382,7 @@
       <c r="E320" s="73"/>
       <c r="F320" s="61"/>
     </row>
-    <row r="321" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A321" s="69"/>
       <c r="B321" s="70"/>
       <c r="C321" s="71"/>
@@ -6381,7 +6390,7 @@
       <c r="E321" s="73"/>
       <c r="F321" s="61"/>
     </row>
-    <row r="322" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A322" s="69"/>
       <c r="B322" s="70"/>
       <c r="C322" s="71"/>
@@ -6389,7 +6398,7 @@
       <c r="E322" s="73"/>
       <c r="F322" s="61"/>
     </row>
-    <row r="323" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A323" s="69"/>
       <c r="B323" s="70"/>
       <c r="C323" s="71"/>
@@ -6397,7 +6406,7 @@
       <c r="E323" s="73"/>
       <c r="F323" s="61"/>
     </row>
-    <row r="324" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A324" s="69"/>
       <c r="B324" s="70"/>
       <c r="C324" s="71"/>
@@ -6405,7 +6414,7 @@
       <c r="E324" s="73"/>
       <c r="F324" s="61"/>
     </row>
-    <row r="325" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A325" s="69"/>
       <c r="B325" s="70"/>
       <c r="C325" s="71"/>
@@ -6413,7 +6422,7 @@
       <c r="E325" s="73"/>
       <c r="F325" s="61"/>
     </row>
-    <row r="326" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A326" s="69"/>
       <c r="B326" s="70"/>
       <c r="C326" s="71"/>
@@ -6421,7 +6430,7 @@
       <c r="E326" s="73"/>
       <c r="F326" s="61"/>
     </row>
-    <row r="327" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A327" s="69"/>
       <c r="B327" s="70"/>
       <c r="C327" s="71"/>
@@ -6429,7 +6438,7 @@
       <c r="E327" s="73"/>
       <c r="F327" s="61"/>
     </row>
-    <row r="328" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A328" s="69"/>
       <c r="B328" s="70"/>
       <c r="C328" s="71"/>
@@ -6437,7 +6446,7 @@
       <c r="E328" s="73"/>
       <c r="F328" s="61"/>
     </row>
-    <row r="329" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A329" s="69"/>
       <c r="B329" s="70"/>
       <c r="C329" s="71"/>
@@ -6445,7 +6454,7 @@
       <c r="E329" s="73"/>
       <c r="F329" s="61"/>
     </row>
-    <row r="330" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A330" s="69"/>
       <c r="B330" s="70"/>
       <c r="C330" s="71"/>
@@ -6453,7 +6462,7 @@
       <c r="E330" s="73"/>
       <c r="F330" s="61"/>
     </row>
-    <row r="331" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A331" s="69"/>
       <c r="B331" s="70"/>
       <c r="C331" s="71"/>
@@ -6461,7 +6470,7 @@
       <c r="E331" s="73"/>
       <c r="F331" s="61"/>
     </row>
-    <row r="332" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A332" s="69"/>
       <c r="B332" s="70"/>
       <c r="C332" s="71"/>
@@ -6469,7 +6478,7 @@
       <c r="E332" s="73"/>
       <c r="F332" s="61"/>
     </row>
-    <row r="333" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A333" s="69"/>
       <c r="B333" s="70"/>
       <c r="C333" s="71"/>
@@ -6477,7 +6486,7 @@
       <c r="E333" s="73"/>
       <c r="F333" s="61"/>
     </row>
-    <row r="334" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A334" s="69"/>
       <c r="B334" s="70"/>
       <c r="C334" s="71"/>
@@ -6485,7 +6494,7 @@
       <c r="E334" s="73"/>
       <c r="F334" s="61"/>
     </row>
-    <row r="335" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A335" s="69"/>
       <c r="B335" s="70"/>
       <c r="C335" s="71"/>
@@ -6493,7 +6502,7 @@
       <c r="E335" s="73"/>
       <c r="F335" s="61"/>
     </row>
-    <row r="336" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A336" s="69"/>
       <c r="B336" s="70"/>
       <c r="C336" s="71"/>
@@ -6501,7 +6510,7 @@
       <c r="E336" s="73"/>
       <c r="F336" s="61"/>
     </row>
-    <row r="337" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A337" s="69"/>
       <c r="B337" s="70"/>
       <c r="C337" s="71"/>
@@ -6509,7 +6518,7 @@
       <c r="E337" s="73"/>
       <c r="F337" s="61"/>
     </row>
-    <row r="338" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A338" s="69"/>
       <c r="B338" s="70"/>
       <c r="C338" s="71"/>
@@ -6517,7 +6526,7 @@
       <c r="E338" s="73"/>
       <c r="F338" s="61"/>
     </row>
-    <row r="339" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A339" s="69"/>
       <c r="B339" s="70"/>
       <c r="C339" s="71"/>
@@ -6525,7 +6534,7 @@
       <c r="E339" s="73"/>
       <c r="F339" s="61"/>
     </row>
-    <row r="340" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A340" s="69"/>
       <c r="B340" s="70"/>
       <c r="C340" s="71"/>
@@ -6533,7 +6542,7 @@
       <c r="E340" s="73"/>
       <c r="F340" s="61"/>
     </row>
-    <row r="341" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A341" s="69"/>
       <c r="B341" s="70"/>
       <c r="C341" s="71"/>
@@ -6541,7 +6550,7 @@
       <c r="E341" s="73"/>
       <c r="F341" s="61"/>
     </row>
-    <row r="342" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A342" s="69"/>
       <c r="B342" s="70"/>
       <c r="C342" s="71"/>
@@ -6549,7 +6558,7 @@
       <c r="E342" s="73"/>
       <c r="F342" s="61"/>
     </row>
-    <row r="343" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A343" s="69"/>
       <c r="B343" s="70"/>
       <c r="C343" s="71"/>
@@ -6557,7 +6566,7 @@
       <c r="E343" s="73"/>
       <c r="F343" s="61"/>
     </row>
-    <row r="344" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A344" s="69"/>
       <c r="B344" s="70"/>
       <c r="C344" s="71"/>
@@ -6565,7 +6574,7 @@
       <c r="E344" s="73"/>
       <c r="F344" s="61"/>
     </row>
-    <row r="345" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A345" s="69"/>
       <c r="B345" s="70"/>
       <c r="C345" s="71"/>
@@ -6573,7 +6582,7 @@
       <c r="E345" s="73"/>
       <c r="F345" s="61"/>
     </row>
-    <row r="346" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A346" s="69"/>
       <c r="B346" s="70"/>
       <c r="C346" s="71"/>
@@ -6581,7 +6590,7 @@
       <c r="E346" s="73"/>
       <c r="F346" s="61"/>
     </row>
-    <row r="347" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A347" s="69"/>
       <c r="B347" s="70"/>
       <c r="C347" s="71"/>
@@ -6589,7 +6598,7 @@
       <c r="E347" s="73"/>
       <c r="F347" s="61"/>
     </row>
-    <row r="348" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A348" s="69"/>
       <c r="B348" s="70"/>
       <c r="C348" s="71"/>
@@ -6597,7 +6606,7 @@
       <c r="E348" s="73"/>
       <c r="F348" s="61"/>
     </row>
-    <row r="349" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A349" s="69"/>
       <c r="B349" s="70"/>
       <c r="C349" s="71"/>
@@ -6605,7 +6614,7 @@
       <c r="E349" s="73"/>
       <c r="F349" s="61"/>
     </row>
-    <row r="350" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A350" s="69"/>
       <c r="B350" s="70"/>
       <c r="C350" s="71"/>
@@ -6613,7 +6622,7 @@
       <c r="E350" s="73"/>
       <c r="F350" s="61"/>
     </row>
-    <row r="351" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A351" s="69"/>
       <c r="B351" s="70"/>
       <c r="C351" s="71"/>
@@ -6621,7 +6630,7 @@
       <c r="E351" s="73"/>
       <c r="F351" s="61"/>
     </row>
-    <row r="352" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A352" s="69"/>
       <c r="B352" s="70"/>
       <c r="C352" s="71"/>
@@ -6629,7 +6638,7 @@
       <c r="E352" s="73"/>
       <c r="F352" s="61"/>
     </row>
-    <row r="353" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A353" s="69"/>
       <c r="B353" s="70"/>
       <c r="C353" s="71"/>
@@ -6637,7 +6646,7 @@
       <c r="E353" s="73"/>
       <c r="F353" s="61"/>
     </row>
-    <row r="354" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A354" s="69"/>
       <c r="B354" s="70"/>
       <c r="C354" s="71"/>
@@ -6645,7 +6654,7 @@
       <c r="E354" s="73"/>
       <c r="F354" s="61"/>
     </row>
-    <row r="355" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A355" s="69"/>
       <c r="B355" s="70"/>
       <c r="C355" s="71"/>
@@ -6653,7 +6662,7 @@
       <c r="E355" s="73"/>
       <c r="F355" s="61"/>
     </row>
-    <row r="356" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A356" s="69"/>
       <c r="B356" s="70"/>
       <c r="C356" s="71"/>
@@ -6661,7 +6670,7 @@
       <c r="E356" s="73"/>
       <c r="F356" s="61"/>
     </row>
-    <row r="357" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A357" s="69"/>
       <c r="B357" s="70"/>
       <c r="C357" s="71"/>
@@ -6669,7 +6678,7 @@
       <c r="E357" s="73"/>
       <c r="F357" s="61"/>
     </row>
-    <row r="358" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A358" s="69"/>
       <c r="B358" s="70"/>
       <c r="C358" s="71"/>
@@ -6677,7 +6686,7 @@
       <c r="E358" s="73"/>
       <c r="F358" s="61"/>
     </row>
-    <row r="359" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A359" s="69"/>
       <c r="B359" s="70"/>
       <c r="C359" s="71"/>
@@ -6685,7 +6694,7 @@
       <c r="E359" s="73"/>
       <c r="F359" s="61"/>
     </row>
-    <row r="360" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A360" s="69"/>
       <c r="B360" s="70"/>
       <c r="C360" s="71"/>
@@ -6693,7 +6702,7 @@
       <c r="E360" s="73"/>
       <c r="F360" s="61"/>
     </row>
-    <row r="361" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A361" s="69"/>
       <c r="B361" s="70"/>
       <c r="C361" s="71"/>
@@ -6701,7 +6710,7 @@
       <c r="E361" s="73"/>
       <c r="F361" s="61"/>
     </row>
-    <row r="362" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A362" s="69"/>
       <c r="B362" s="70"/>
       <c r="C362" s="71"/>
@@ -6709,7 +6718,7 @@
       <c r="E362" s="73"/>
       <c r="F362" s="61"/>
     </row>
-    <row r="363" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A363" s="69"/>
       <c r="B363" s="70"/>
       <c r="C363" s="71"/>
@@ -6717,7 +6726,7 @@
       <c r="E363" s="73"/>
       <c r="F363" s="61"/>
     </row>
-    <row r="364" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A364" s="69"/>
       <c r="B364" s="70"/>
       <c r="C364" s="71"/>
@@ -6725,7 +6734,7 @@
       <c r="E364" s="73"/>
       <c r="F364" s="61"/>
     </row>
-    <row r="365" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A365" s="69"/>
       <c r="B365" s="70"/>
       <c r="C365" s="71"/>
@@ -6733,7 +6742,7 @@
       <c r="E365" s="73"/>
       <c r="F365" s="61"/>
     </row>
-    <row r="366" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A366" s="69"/>
       <c r="B366" s="70"/>
       <c r="C366" s="71"/>
@@ -6741,7 +6750,7 @@
       <c r="E366" s="73"/>
       <c r="F366" s="61"/>
     </row>
-    <row r="367" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A367" s="69"/>
       <c r="B367" s="70"/>
       <c r="C367" s="71"/>
@@ -6749,7 +6758,7 @@
       <c r="E367" s="73"/>
       <c r="F367" s="61"/>
     </row>
-    <row r="368" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A368" s="69"/>
       <c r="B368" s="70"/>
       <c r="C368" s="71"/>
@@ -6757,7 +6766,7 @@
       <c r="E368" s="73"/>
       <c r="F368" s="61"/>
     </row>
-    <row r="369" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A369" s="69"/>
       <c r="B369" s="70"/>
       <c r="C369" s="71"/>
@@ -6765,7 +6774,7 @@
       <c r="E369" s="73"/>
       <c r="F369" s="61"/>
     </row>
-    <row r="370" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A370" s="69"/>
       <c r="B370" s="70"/>
       <c r="C370" s="71"/>
@@ -6773,7 +6782,7 @@
       <c r="E370" s="73"/>
       <c r="F370" s="61"/>
     </row>
-    <row r="371" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A371" s="69"/>
       <c r="B371" s="70"/>
       <c r="C371" s="71"/>
@@ -6781,7 +6790,7 @@
       <c r="E371" s="73"/>
       <c r="F371" s="61"/>
     </row>
-    <row r="372" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A372" s="69"/>
       <c r="B372" s="70"/>
       <c r="C372" s="71"/>
@@ -6789,7 +6798,7 @@
       <c r="E372" s="73"/>
       <c r="F372" s="61"/>
     </row>
-    <row r="373" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A373" s="69"/>
       <c r="B373" s="70"/>
       <c r="C373" s="71"/>
@@ -6797,7 +6806,7 @@
       <c r="E373" s="73"/>
       <c r="F373" s="61"/>
     </row>
-    <row r="374" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A374" s="69"/>
       <c r="B374" s="70"/>
       <c r="C374" s="71"/>
@@ -6805,7 +6814,7 @@
       <c r="E374" s="73"/>
       <c r="F374" s="61"/>
     </row>
-    <row r="375" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A375" s="69"/>
       <c r="B375" s="70"/>
       <c r="C375" s="71"/>
@@ -6813,7 +6822,7 @@
       <c r="E375" s="73"/>
       <c r="F375" s="61"/>
     </row>
-    <row r="376" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A376" s="69"/>
       <c r="B376" s="70"/>
       <c r="C376" s="71"/>
@@ -6821,7 +6830,7 @@
       <c r="E376" s="73"/>
       <c r="F376" s="61"/>
     </row>
-    <row r="377" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A377" s="69"/>
       <c r="B377" s="70"/>
       <c r="C377" s="71"/>
@@ -6829,7 +6838,7 @@
       <c r="E377" s="73"/>
       <c r="F377" s="61"/>
     </row>
-    <row r="378" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A378" s="69"/>
       <c r="B378" s="70"/>
       <c r="C378" s="71"/>
@@ -6837,7 +6846,7 @@
       <c r="E378" s="73"/>
       <c r="F378" s="61"/>
     </row>
-    <row r="379" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A379" s="69"/>
       <c r="B379" s="70"/>
       <c r="C379" s="71"/>
@@ -6845,7 +6854,7 @@
       <c r="E379" s="73"/>
       <c r="F379" s="61"/>
     </row>
-    <row r="380" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A380" s="69"/>
       <c r="B380" s="70"/>
       <c r="C380" s="71"/>
@@ -6853,7 +6862,7 @@
       <c r="E380" s="73"/>
       <c r="F380" s="61"/>
     </row>
-    <row r="381" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A381" s="69"/>
       <c r="B381" s="70"/>
       <c r="C381" s="71"/>
@@ -6861,7 +6870,7 @@
       <c r="E381" s="73"/>
       <c r="F381" s="61"/>
     </row>
-    <row r="382" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A382" s="69"/>
       <c r="B382" s="70"/>
       <c r="C382" s="71"/>
@@ -6869,7 +6878,7 @@
       <c r="E382" s="73"/>
       <c r="F382" s="61"/>
     </row>
-    <row r="383" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A383" s="69"/>
       <c r="B383" s="70"/>
       <c r="C383" s="71"/>
@@ -6877,7 +6886,7 @@
       <c r="E383" s="73"/>
       <c r="F383" s="61"/>
     </row>
-    <row r="384" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A384" s="69"/>
       <c r="B384" s="70"/>
       <c r="C384" s="71"/>
@@ -6885,7 +6894,7 @@
       <c r="E384" s="73"/>
       <c r="F384" s="61"/>
     </row>
-    <row r="385" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A385" s="69"/>
       <c r="B385" s="70"/>
       <c r="C385" s="71"/>
@@ -6893,7 +6902,7 @@
       <c r="E385" s="73"/>
       <c r="F385" s="61"/>
     </row>
-    <row r="386" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A386" s="69"/>
       <c r="B386" s="70"/>
       <c r="C386" s="71"/>
@@ -6901,7 +6910,7 @@
       <c r="E386" s="73"/>
       <c r="F386" s="61"/>
     </row>
-    <row r="387" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A387" s="69"/>
       <c r="B387" s="70"/>
       <c r="C387" s="71"/>
@@ -6909,7 +6918,7 @@
       <c r="E387" s="73"/>
       <c r="F387" s="61"/>
     </row>
-    <row r="388" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A388" s="69"/>
       <c r="B388" s="70"/>
       <c r="C388" s="71"/>
@@ -6917,7 +6926,7 @@
       <c r="E388" s="73"/>
       <c r="F388" s="61"/>
     </row>
-    <row r="389" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A389" s="69"/>
       <c r="B389" s="70"/>
       <c r="C389" s="71"/>
@@ -6925,7 +6934,7 @@
       <c r="E389" s="73"/>
       <c r="F389" s="61"/>
     </row>
-    <row r="390" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A390" s="69"/>
       <c r="B390" s="70"/>
       <c r="C390" s="71"/>
@@ -6933,7 +6942,7 @@
       <c r="E390" s="73"/>
       <c r="F390" s="61"/>
     </row>
-    <row r="391" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A391" s="69"/>
       <c r="B391" s="70"/>
       <c r="C391" s="71"/>
@@ -6941,7 +6950,7 @@
       <c r="E391" s="73"/>
       <c r="F391" s="61"/>
     </row>
-    <row r="392" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A392" s="69"/>
       <c r="B392" s="70"/>
       <c r="C392" s="71"/>
@@ -6949,7 +6958,7 @@
       <c r="E392" s="73"/>
       <c r="F392" s="61"/>
     </row>
-    <row r="393" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A393" s="69"/>
       <c r="B393" s="70"/>
       <c r="C393" s="71"/>
@@ -6957,7 +6966,7 @@
       <c r="E393" s="73"/>
       <c r="F393" s="61"/>
     </row>
-    <row r="394" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A394" s="69"/>
       <c r="B394" s="70"/>
       <c r="C394" s="71"/>
@@ -6965,7 +6974,7 @@
       <c r="E394" s="73"/>
       <c r="F394" s="61"/>
     </row>
-    <row r="395" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A395" s="69"/>
       <c r="B395" s="70"/>
       <c r="C395" s="71"/>
@@ -6973,7 +6982,7 @@
       <c r="E395" s="73"/>
       <c r="F395" s="61"/>
     </row>
-    <row r="396" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A396" s="69"/>
       <c r="B396" s="70"/>
       <c r="C396" s="71"/>
@@ -6981,7 +6990,7 @@
       <c r="E396" s="73"/>
       <c r="F396" s="61"/>
     </row>
-    <row r="397" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A397" s="69"/>
       <c r="B397" s="70"/>
       <c r="C397" s="71"/>
@@ -6989,7 +6998,7 @@
       <c r="E397" s="73"/>
       <c r="F397" s="61"/>
     </row>
-    <row r="398" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A398" s="69"/>
       <c r="B398" s="70"/>
       <c r="C398" s="71"/>
@@ -6997,7 +7006,7 @@
       <c r="E398" s="73"/>
       <c r="F398" s="61"/>
     </row>
-    <row r="399" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A399" s="69"/>
       <c r="B399" s="70"/>
       <c r="C399" s="71"/>
@@ -7005,7 +7014,7 @@
       <c r="E399" s="73"/>
       <c r="F399" s="61"/>
     </row>
-    <row r="400" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A400" s="69"/>
       <c r="B400" s="70"/>
       <c r="C400" s="71"/>
@@ -7013,7 +7022,7 @@
       <c r="E400" s="73"/>
       <c r="F400" s="61"/>
     </row>
-    <row r="401" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A401" s="69"/>
       <c r="B401" s="70"/>
       <c r="C401" s="71"/>
@@ -7021,7 +7030,7 @@
       <c r="E401" s="73"/>
       <c r="F401" s="61"/>
     </row>
-    <row r="402" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A402" s="69"/>
       <c r="B402" s="70"/>
       <c r="C402" s="71"/>
@@ -7029,7 +7038,7 @@
       <c r="E402" s="73"/>
       <c r="F402" s="61"/>
     </row>
-    <row r="403" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A403" s="69"/>
       <c r="B403" s="70"/>
       <c r="C403" s="71"/>
@@ -7037,7 +7046,7 @@
       <c r="E403" s="73"/>
       <c r="F403" s="61"/>
     </row>
-    <row r="404" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A404" s="69"/>
       <c r="B404" s="70"/>
       <c r="C404" s="71"/>
@@ -7045,17 +7054,17 @@
       <c r="E404" s="73"/>
       <c r="F404" s="61"/>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A405" s="47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A406" s="74" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="407" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A407" s="75">
         <v>2</v>
       </c>

</xml_diff>